<commit_message>
fix: magic - 20220421
</commit_message>
<xml_diff>
--- a/magic_excel.xlsx
+++ b/magic_excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13000" yWindow="0" windowWidth="22320" windowHeight="19400"/>
+    <workbookView xWindow="11200" yWindow="0" windowWidth="22320" windowHeight="19400"/>
   </bookViews>
   <sheets>
     <sheet name="图" sheetId="3" r:id="rId1"/>
@@ -2217,15 +2217,18 @@
                 <c:pt idx="335">
                   <c:v>44671.0</c:v>
                 </c:pt>
+                <c:pt idx="336">
+                  <c:v>44672.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$T$2:$T$337</c:f>
+              <c:f>情绪数据!$T$2:$T$338</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="336"/>
+                <c:ptCount val="337"/>
                 <c:pt idx="0">
                   <c:v>4.0</c:v>
                 </c:pt>
@@ -3232,6 +3235,9 @@
                   <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="335">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="336">
                   <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3247,8 +3253,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2101846808"/>
-        <c:axId val="2100368984"/>
+        <c:axId val="-2131811416"/>
+        <c:axId val="-2132100104"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4325,10 +4331,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$U$2:$U$337</c:f>
+              <c:f>情绪数据!$U$2:$U$338</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="336"/>
+                <c:ptCount val="337"/>
                 <c:pt idx="0">
                   <c:v>3.0</c:v>
                 </c:pt>
@@ -5335,6 +5341,9 @@
                   <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="335">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="336">
                   <c:v>4.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -5352,8 +5361,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2101846808"/>
-        <c:axId val="2100368984"/>
+        <c:axId val="-2131811416"/>
+        <c:axId val="-2132100104"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6388,10 +6397,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$J$2:$J$337</c:f>
+              <c:f>情绪数据!$J$2:$J$338</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="336"/>
+                <c:ptCount val="337"/>
                 <c:pt idx="0">
                   <c:v>1.8</c:v>
                 </c:pt>
@@ -7399,6 +7408,9 @@
                 </c:pt>
                 <c:pt idx="335">
                   <c:v>2.14</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>-0.86</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8449,10 +8461,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$K$2:$K$337</c:f>
+              <c:f>情绪数据!$K$2:$K$338</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="336"/>
+                <c:ptCount val="337"/>
                 <c:pt idx="0">
                   <c:v>-0.54</c:v>
                 </c:pt>
@@ -9460,6 +9472,9 @@
                 </c:pt>
                 <c:pt idx="335">
                   <c:v>1.16</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>-1.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9476,11 +9491,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2100365608"/>
-        <c:axId val="2100363544"/>
+        <c:axId val="-2132096376"/>
+        <c:axId val="-2132093432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2101846808"/>
+        <c:axId val="-2131811416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9548,7 +9563,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2100368984"/>
+        <c:crossAx val="-2132100104"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -9556,7 +9571,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100368984"/>
+        <c:axId val="-2132100104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9607,13 +9622,13 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2101846808"/>
+        <c:crossAx val="-2131811416"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2100365608"/>
+        <c:axId val="-2132096376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9623,7 +9638,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100363544"/>
+        <c:crossAx val="-2132093432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -9631,7 +9646,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100363544"/>
+        <c:axId val="-2132093432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9668,7 +9683,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2100365608"/>
+        <c:crossAx val="-2132096376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10784,15 +10799,18 @@
                 <c:pt idx="335">
                   <c:v>44671.0</c:v>
                 </c:pt>
+                <c:pt idx="336">
+                  <c:v>44672.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$B$2:$B$337</c:f>
+              <c:f>情绪数据!$B$2:$B$338</c:f>
               <c:numCache>
                 <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
-                <c:ptCount val="336"/>
+                <c:ptCount val="337"/>
                 <c:pt idx="0">
                   <c:v>26.0</c:v>
                 </c:pt>
@@ -11800,6 +11818,9 @@
                 </c:pt>
                 <c:pt idx="335">
                   <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12845,15 +12866,18 @@
                 <c:pt idx="335">
                   <c:v>44671.0</c:v>
                 </c:pt>
+                <c:pt idx="336">
+                  <c:v>44672.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$C$2:$C$337</c:f>
+              <c:f>情绪数据!$C$2:$C$338</c:f>
               <c:numCache>
                 <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
-                <c:ptCount val="336"/>
+                <c:ptCount val="337"/>
                 <c:pt idx="0">
                   <c:v>30.0</c:v>
                 </c:pt>
@@ -13861,6 +13885,9 @@
                 </c:pt>
                 <c:pt idx="335">
                   <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>15.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13874,8 +13901,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2099454920"/>
-        <c:axId val="2101936696"/>
+        <c:axId val="-2134481848"/>
+        <c:axId val="-2134477992"/>
       </c:areaChart>
       <c:areaChart>
         <c:grouping val="stacked"/>
@@ -14894,10 +14921,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$D$2:$D$337</c:f>
+              <c:f>情绪数据!$D$2:$D$338</c:f>
               <c:numCache>
                 <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
-                <c:ptCount val="336"/>
+                <c:ptCount val="337"/>
                 <c:pt idx="0">
                   <c:v>-17.0</c:v>
                 </c:pt>
@@ -15905,6 +15932,9 @@
                 </c:pt>
                 <c:pt idx="335">
                   <c:v>-19.0</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>-90.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16925,10 +16955,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$F$2:$F$337</c:f>
+              <c:f>情绪数据!$F$2:$F$338</c:f>
               <c:numCache>
                 <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
-                <c:ptCount val="336"/>
+                <c:ptCount val="337"/>
                 <c:pt idx="0">
                   <c:v>-158.0</c:v>
                 </c:pt>
@@ -17936,6 +17966,9 @@
                 </c:pt>
                 <c:pt idx="335">
                   <c:v>-408.0</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>-1963.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17949,8 +17982,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2101940424"/>
-        <c:axId val="2101943400"/>
+        <c:axId val="-2134474264"/>
+        <c:axId val="-2134471288"/>
       </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -18970,10 +19003,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$AF$2:$AF$337</c:f>
+              <c:f>情绪数据!$AF$2:$AF$338</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="336"/>
+                <c:ptCount val="337"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -19981,6 +20014,9 @@
                 </c:pt>
                 <c:pt idx="335">
                   <c:v>56.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>61.33333333333334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19997,11 +20033,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2099454920"/>
-        <c:axId val="2101936696"/>
+        <c:axId val="-2134481848"/>
+        <c:axId val="-2134477992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2099454920"/>
+        <c:axId val="-2134481848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20055,7 +20091,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2101936696"/>
+        <c:crossAx val="-2134477992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -20063,7 +20099,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2101936696"/>
+        <c:axId val="-2134477992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="350.0"/>
@@ -20112,12 +20148,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2099454920"/>
+        <c:crossAx val="-2134481848"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2101940424"/>
+        <c:axId val="-2134474264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20127,7 +20163,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101943400"/>
+        <c:crossAx val="-2134471288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -20135,7 +20171,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2101943400"/>
+        <c:axId val="-2134471288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.0"/>
@@ -20171,7 +20207,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2101940424"/>
+        <c:crossAx val="-2134474264"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21648,8 +21684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="T33:CZ70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BP1" zoomScale="90" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="BZ25" sqref="BZ25"/>
+    <sheetView tabSelected="1" topLeftCell="BL2" zoomScale="90" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="BZ16" sqref="BZ16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -21692,11 +21728,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG337"/>
+  <dimension ref="A1:AG338"/>
   <sheetViews>
     <sheetView zoomScale="117" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T339" sqref="T339"/>
+      <selection pane="bottomLeft" activeCell="K340" sqref="K340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -35615,7 +35651,7 @@
         <v>-250</v>
       </c>
       <c r="I272" s="97">
-        <f t="shared" ref="I272:I337" si="26">B272/(B272+C272)*100</f>
+        <f t="shared" ref="I272:I338" si="26">B272/(B272+C272)*100</f>
         <v>81.395348837209298</v>
       </c>
       <c r="J272" s="97">
@@ -39335,6 +39371,56 @@
       <c r="AG337" s="110">
         <f t="shared" ref="AG337" si="50">(B337-AF337)/AF337</f>
         <v>-8.2352941176470545E-2</v>
+      </c>
+    </row>
+    <row r="338" spans="1:33">
+      <c r="A338" s="37">
+        <v>44672</v>
+      </c>
+      <c r="B338" s="38">
+        <v>32</v>
+      </c>
+      <c r="C338" s="38">
+        <v>15</v>
+      </c>
+      <c r="D338" s="38">
+        <v>-90</v>
+      </c>
+      <c r="E338" s="38">
+        <v>-66</v>
+      </c>
+      <c r="F338" s="38">
+        <v>-1963</v>
+      </c>
+      <c r="G338" s="38">
+        <v>-1344</v>
+      </c>
+      <c r="H338" s="38">
+        <v>-250</v>
+      </c>
+      <c r="I338" s="39">
+        <f t="shared" si="26"/>
+        <v>68.085106382978722</v>
+      </c>
+      <c r="J338" s="39">
+        <v>-0.86</v>
+      </c>
+      <c r="K338" s="39">
+        <v>-1.85</v>
+      </c>
+      <c r="T338" s="94">
+        <v>5</v>
+      </c>
+      <c r="U338" s="43">
+        <v>4</v>
+      </c>
+      <c r="AF338" s="109">
+        <f t="shared" ref="AF338" si="51">(B335+B336+B337)/3</f>
+        <v>61.333333333333336</v>
+      </c>
+      <c r="AG338" s="110">
+        <f t="shared" ref="AG338" si="52">(B338-AF338)/AF338</f>
+        <v>-0.47826086956521741</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: magic&date - 20220423
</commit_message>
<xml_diff>
--- a/magic_excel.xlsx
+++ b/magic_excel.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newhope_ghost/Documents/codeDir/github/stockDetailQuery/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13000" yWindow="0" windowWidth="22320" windowHeight="19400"/>
+    <workbookView xWindow="14800" yWindow="460" windowWidth="20520" windowHeight="19400"/>
   </bookViews>
   <sheets>
     <sheet name="图" sheetId="3" r:id="rId1"/>
     <sheet name="情绪数据" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="8" state="hidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -454,12 +459,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="0.00_ "/>
-    <numFmt numFmtId="178" formatCode="0_ ;[Red]\-0\ "/>
-    <numFmt numFmtId="179" formatCode="0.00_ ;[Red]\-0.00\ "/>
-    <numFmt numFmtId="180" formatCode="0.0%"/>
-    <numFmt numFmtId="181" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="0_ ;[Red]\-0\ "/>
+    <numFmt numFmtId="178" formatCode="0.00_ ;[Red]\-0.00\ "/>
+    <numFmt numFmtId="179" formatCode="0.0%"/>
+    <numFmt numFmtId="180" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="31" x14ac:knownFonts="1">
     <font>
@@ -831,7 +836,7 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -914,26 +919,26 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="178" fontId="0" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="0" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="28" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -946,66 +951,66 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="178" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="178" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="178" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="178" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="178" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="178" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="16" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="16" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="18" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="18" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="178" fontId="18" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="18" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1017,57 +1022,57 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="18" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="18" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="18" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="18" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="18" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="0" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="179" fontId="18" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="2" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="0" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="178" fontId="18" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="2" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="百分比" xfId="1" builtinId="5"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="逗号" xfId="8" builtinId="3"/>
-    <cellStyle name="访问过的超链接" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2217,15 +2222,21 @@
                 <c:pt idx="335">
                   <c:v>44671.0</c:v>
                 </c:pt>
+                <c:pt idx="336">
+                  <c:v>44672.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>44673.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$T$2:$T$337</c:f>
+              <c:f>情绪数据!$T$2:$T$339</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="336"/>
+                <c:ptCount val="338"/>
                 <c:pt idx="0">
                   <c:v>4.0</c:v>
                 </c:pt>
@@ -3232,6 +3243,12 @@
                   <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="335">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
                   <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -3247,8 +3264,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2101846808"/>
-        <c:axId val="2100368984"/>
+        <c:axId val="-849261504"/>
+        <c:axId val="-849259728"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4325,10 +4342,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$U$2:$U$337</c:f>
+              <c:f>情绪数据!$U$2:$U$339</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="336"/>
+                <c:ptCount val="338"/>
                 <c:pt idx="0">
                   <c:v>3.0</c:v>
                 </c:pt>
@@ -5336,6 +5353,12 @@
                 </c:pt>
                 <c:pt idx="335">
                   <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5352,8 +5375,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2101846808"/>
-        <c:axId val="2100368984"/>
+        <c:axId val="-849261504"/>
+        <c:axId val="-849259728"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6388,10 +6411,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$J$2:$J$337</c:f>
+              <c:f>情绪数据!$J$2:$J$339</c:f>
               <c:numCache>
-                <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="336"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="338"/>
                 <c:pt idx="0">
                   <c:v>1.8</c:v>
                 </c:pt>
@@ -7399,6 +7422,12 @@
                 </c:pt>
                 <c:pt idx="335">
                   <c:v>2.14</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>-0.86</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>2.63</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8449,10 +8478,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$K$2:$K$337</c:f>
+              <c:f>情绪数据!$K$2:$K$339</c:f>
               <c:numCache>
-                <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="336"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="338"/>
                 <c:pt idx="0">
                   <c:v>-0.54</c:v>
                 </c:pt>
@@ -9460,6 +9489,12 @@
                 </c:pt>
                 <c:pt idx="335">
                   <c:v>1.16</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>-1.85</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>0.19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9476,11 +9511,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2100365608"/>
-        <c:axId val="2100363544"/>
+        <c:axId val="-849257408"/>
+        <c:axId val="-849255088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2101846808"/>
+        <c:axId val="-849261504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9548,7 +9583,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2100368984"/>
+        <c:crossAx val="-849259728"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -9556,7 +9591,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100368984"/>
+        <c:axId val="-849259728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9607,13 +9642,13 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2101846808"/>
+        <c:crossAx val="-849261504"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2100365608"/>
+        <c:axId val="-849257408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9623,7 +9658,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100363544"/>
+        <c:crossAx val="-849255088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -9631,7 +9666,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100363544"/>
+        <c:axId val="-849255088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9668,7 +9703,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2100365608"/>
+        <c:crossAx val="-849257408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10784,15 +10819,21 @@
                 <c:pt idx="335">
                   <c:v>44671.0</c:v>
                 </c:pt>
+                <c:pt idx="336">
+                  <c:v>44672.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>44673.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$B$2:$B$337</c:f>
+              <c:f>情绪数据!$B$2:$B$339</c:f>
               <c:numCache>
-                <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
-                <c:ptCount val="336"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="338"/>
                 <c:pt idx="0">
                   <c:v>26.0</c:v>
                 </c:pt>
@@ -11648,85 +11689,85 @@
                 <c:pt idx="284">
                   <c:v>56.0</c:v>
                 </c:pt>
-                <c:pt idx="285" formatCode="General">
+                <c:pt idx="285">
                   <c:v>86.0</c:v>
                 </c:pt>
-                <c:pt idx="286" formatCode="General">
+                <c:pt idx="286">
                   <c:v>97.0</c:v>
                 </c:pt>
-                <c:pt idx="287" formatCode="General">
+                <c:pt idx="287">
                   <c:v>96.0</c:v>
                 </c:pt>
-                <c:pt idx="288" formatCode="General">
+                <c:pt idx="288">
                   <c:v>56.0</c:v>
                 </c:pt>
-                <c:pt idx="289" formatCode="General">
+                <c:pt idx="289">
                   <c:v>51.0</c:v>
                 </c:pt>
-                <c:pt idx="290" formatCode="General">
+                <c:pt idx="290">
                   <c:v>84.0</c:v>
                 </c:pt>
-                <c:pt idx="291" formatCode="General">
+                <c:pt idx="291">
                   <c:v>56.0</c:v>
                 </c:pt>
-                <c:pt idx="292" formatCode="General">
+                <c:pt idx="292">
                   <c:v>72.0</c:v>
                 </c:pt>
-                <c:pt idx="293" formatCode="General">
+                <c:pt idx="293">
                   <c:v>45.0</c:v>
                 </c:pt>
-                <c:pt idx="294" formatCode="General">
+                <c:pt idx="294">
                   <c:v>52.0</c:v>
                 </c:pt>
-                <c:pt idx="295" formatCode="General">
+                <c:pt idx="295">
                   <c:v>100.0</c:v>
                 </c:pt>
-                <c:pt idx="296" formatCode="General">
+                <c:pt idx="296">
                   <c:v>51.0</c:v>
                 </c:pt>
-                <c:pt idx="297" formatCode="General">
+                <c:pt idx="297">
                   <c:v>89.0</c:v>
                 </c:pt>
-                <c:pt idx="298" formatCode="General">
+                <c:pt idx="298">
                   <c:v>38.0</c:v>
                 </c:pt>
-                <c:pt idx="299" formatCode="General">
+                <c:pt idx="299">
                   <c:v>60.0</c:v>
                 </c:pt>
-                <c:pt idx="300" formatCode="General">
+                <c:pt idx="300">
                   <c:v>45.0</c:v>
                 </c:pt>
-                <c:pt idx="301" formatCode="General">
+                <c:pt idx="301">
                   <c:v>53.0</c:v>
                 </c:pt>
-                <c:pt idx="302" formatCode="General">
+                <c:pt idx="302">
                   <c:v>64.0</c:v>
                 </c:pt>
-                <c:pt idx="303" formatCode="General">
+                <c:pt idx="303">
                   <c:v>76.0</c:v>
                 </c:pt>
-                <c:pt idx="304" formatCode="General">
+                <c:pt idx="304">
                   <c:v>45.0</c:v>
                 </c:pt>
-                <c:pt idx="305" formatCode="General">
+                <c:pt idx="305">
                   <c:v>52.0</c:v>
                 </c:pt>
-                <c:pt idx="306" formatCode="General">
+                <c:pt idx="306">
                   <c:v>21.0</c:v>
                 </c:pt>
-                <c:pt idx="307" formatCode="General">
+                <c:pt idx="307">
                   <c:v>46.0</c:v>
                 </c:pt>
-                <c:pt idx="308" formatCode="General">
+                <c:pt idx="308">
                   <c:v>84.0</c:v>
                 </c:pt>
-                <c:pt idx="309" formatCode="General">
+                <c:pt idx="309">
                   <c:v>69.0</c:v>
                 </c:pt>
-                <c:pt idx="310" formatCode="General">
+                <c:pt idx="310">
                   <c:v>43.0</c:v>
                 </c:pt>
-                <c:pt idx="311" formatCode="General">
+                <c:pt idx="311">
                   <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="312">
@@ -11759,16 +11800,16 @@
                 <c:pt idx="321">
                   <c:v>56.0</c:v>
                 </c:pt>
-                <c:pt idx="322" formatCode="General">
+                <c:pt idx="322">
                   <c:v>80.0</c:v>
                 </c:pt>
-                <c:pt idx="323" formatCode="General">
+                <c:pt idx="323">
                   <c:v>55.0</c:v>
                 </c:pt>
-                <c:pt idx="324" formatCode="General">
+                <c:pt idx="324">
                   <c:v>72.0</c:v>
                 </c:pt>
-                <c:pt idx="325" formatCode="General">
+                <c:pt idx="325">
                   <c:v>82.0</c:v>
                 </c:pt>
                 <c:pt idx="326">
@@ -11800,6 +11841,12 @@
                 </c:pt>
                 <c:pt idx="335">
                   <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>75.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12845,15 +12892,21 @@
                 <c:pt idx="335">
                   <c:v>44671.0</c:v>
                 </c:pt>
+                <c:pt idx="336">
+                  <c:v>44672.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>44673.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$C$2:$C$337</c:f>
+              <c:f>情绪数据!$C$2:$C$339</c:f>
               <c:numCache>
-                <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
-                <c:ptCount val="336"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="338"/>
                 <c:pt idx="0">
                   <c:v>30.0</c:v>
                 </c:pt>
@@ -13709,85 +13762,85 @@
                 <c:pt idx="284">
                   <c:v>22.0</c:v>
                 </c:pt>
-                <c:pt idx="285" formatCode="General">
+                <c:pt idx="285">
                   <c:v>26.0</c:v>
                 </c:pt>
-                <c:pt idx="286" formatCode="General">
+                <c:pt idx="286">
                   <c:v>19.0</c:v>
                 </c:pt>
-                <c:pt idx="287" formatCode="General">
+                <c:pt idx="287">
                   <c:v>19.0</c:v>
                 </c:pt>
-                <c:pt idx="288" formatCode="General">
+                <c:pt idx="288">
                   <c:v>25.0</c:v>
                 </c:pt>
-                <c:pt idx="289" formatCode="General">
+                <c:pt idx="289">
                   <c:v>17.0</c:v>
                 </c:pt>
-                <c:pt idx="290" formatCode="General">
+                <c:pt idx="290">
                   <c:v>28.0</c:v>
                 </c:pt>
-                <c:pt idx="291" formatCode="General">
+                <c:pt idx="291">
                   <c:v>31.0</c:v>
                 </c:pt>
-                <c:pt idx="292" formatCode="General">
+                <c:pt idx="292">
                   <c:v>26.0</c:v>
                 </c:pt>
-                <c:pt idx="293" formatCode="General">
+                <c:pt idx="293">
                   <c:v>41.0</c:v>
                 </c:pt>
-                <c:pt idx="294" formatCode="General">
+                <c:pt idx="294">
                   <c:v>19.0</c:v>
                 </c:pt>
-                <c:pt idx="295" formatCode="General">
+                <c:pt idx="295">
                   <c:v>17.0</c:v>
                 </c:pt>
-                <c:pt idx="296" formatCode="General">
+                <c:pt idx="296">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="297" formatCode="General">
+                <c:pt idx="297">
                   <c:v>20.0</c:v>
                 </c:pt>
-                <c:pt idx="298" formatCode="General">
+                <c:pt idx="298">
                   <c:v>36.0</c:v>
                 </c:pt>
-                <c:pt idx="299" formatCode="General">
+                <c:pt idx="299">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="300" formatCode="General">
+                <c:pt idx="300">
                   <c:v>22.0</c:v>
                 </c:pt>
-                <c:pt idx="301" formatCode="General">
+                <c:pt idx="301">
                   <c:v>16.0</c:v>
                 </c:pt>
-                <c:pt idx="302" formatCode="General">
+                <c:pt idx="302">
                   <c:v>13.0</c:v>
                 </c:pt>
-                <c:pt idx="303" formatCode="General">
+                <c:pt idx="303">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="304" formatCode="General">
+                <c:pt idx="304">
                   <c:v>25.0</c:v>
                 </c:pt>
-                <c:pt idx="305" formatCode="General">
+                <c:pt idx="305">
                   <c:v>19.0</c:v>
                 </c:pt>
-                <c:pt idx="306" formatCode="General">
+                <c:pt idx="306">
                   <c:v>33.0</c:v>
                 </c:pt>
-                <c:pt idx="307" formatCode="General">
+                <c:pt idx="307">
                   <c:v>22.0</c:v>
                 </c:pt>
-                <c:pt idx="308" formatCode="General">
+                <c:pt idx="308">
                   <c:v>39.0</c:v>
                 </c:pt>
-                <c:pt idx="309" formatCode="General">
+                <c:pt idx="309">
                   <c:v>18.0</c:v>
                 </c:pt>
-                <c:pt idx="310" formatCode="General">
+                <c:pt idx="310">
                   <c:v>25.0</c:v>
                 </c:pt>
-                <c:pt idx="311" formatCode="General">
+                <c:pt idx="311">
                   <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="312">
@@ -13820,16 +13873,16 @@
                 <c:pt idx="321">
                   <c:v>23.0</c:v>
                 </c:pt>
-                <c:pt idx="322" formatCode="General">
+                <c:pt idx="322">
                   <c:v>28.0</c:v>
                 </c:pt>
-                <c:pt idx="323" formatCode="General">
+                <c:pt idx="323">
                   <c:v>48.0</c:v>
                 </c:pt>
-                <c:pt idx="324" formatCode="General">
+                <c:pt idx="324">
                   <c:v>12.0</c:v>
                 </c:pt>
-                <c:pt idx="325" formatCode="General">
+                <c:pt idx="325">
                   <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="326">
@@ -13861,6 +13914,12 @@
                 </c:pt>
                 <c:pt idx="335">
                   <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>10.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13874,8 +13933,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2099454920"/>
-        <c:axId val="2101936696"/>
+        <c:axId val="-848938144"/>
+        <c:axId val="-848935824"/>
       </c:areaChart>
       <c:areaChart>
         <c:grouping val="stacked"/>
@@ -14894,10 +14953,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$D$2:$D$337</c:f>
+              <c:f>情绪数据!$D$2:$D$339</c:f>
               <c:numCache>
-                <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
-                <c:ptCount val="336"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="338"/>
                 <c:pt idx="0">
                   <c:v>-17.0</c:v>
                 </c:pt>
@@ -15905,6 +15964,12 @@
                 </c:pt>
                 <c:pt idx="335">
                   <c:v>-19.0</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>-90.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>-85.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16925,10 +16990,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$F$2:$F$337</c:f>
+              <c:f>情绪数据!$F$2:$F$339</c:f>
               <c:numCache>
-                <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
-                <c:ptCount val="336"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="338"/>
                 <c:pt idx="0">
                   <c:v>-158.0</c:v>
                 </c:pt>
@@ -17936,6 +18001,12 @@
                 </c:pt>
                 <c:pt idx="335">
                   <c:v>-408.0</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>-1963.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>-665.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17949,8 +18020,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2101940424"/>
-        <c:axId val="2101943400"/>
+        <c:axId val="-848933504"/>
+        <c:axId val="-848931184"/>
       </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -18970,10 +19041,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$AF$2:$AF$337</c:f>
+              <c:f>情绪数据!$AF$2:$AF$339</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="336"/>
+                <c:ptCount val="338"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -19981,6 +20052,12 @@
                 </c:pt>
                 <c:pt idx="335">
                   <c:v>56.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>61.33333333333334</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>46.66666666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19997,11 +20074,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2099454920"/>
-        <c:axId val="2101936696"/>
+        <c:axId val="-848938144"/>
+        <c:axId val="-848935824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2099454920"/>
+        <c:axId val="-848938144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20055,7 +20132,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2101936696"/>
+        <c:crossAx val="-848935824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -20063,7 +20140,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2101936696"/>
+        <c:axId val="-848935824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="350.0"/>
@@ -20112,12 +20189,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2099454920"/>
+        <c:crossAx val="-848938144"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2101940424"/>
+        <c:axId val="-848933504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20127,7 +20204,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101943400"/>
+        <c:crossAx val="-848931184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -20135,7 +20212,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2101943400"/>
+        <c:axId val="-848931184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.0"/>
@@ -20171,7 +20248,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2101940424"/>
+        <c:crossAx val="-848933504"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21648,31 +21725,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="T33:CZ70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BP1" zoomScale="90" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="BZ25" sqref="BZ25"/>
+    <sheetView tabSelected="1" topLeftCell="BK1" zoomScale="88" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="CD21" sqref="CD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="33" spans="97:104">
+    <row r="33" spans="97:104" x14ac:dyDescent="0.2">
       <c r="CY33" s="18"/>
     </row>
-    <row r="34" spans="97:104">
+    <row r="34" spans="97:104" x14ac:dyDescent="0.2">
       <c r="CS34" s="18"/>
     </row>
-    <row r="37" spans="97:104" ht="15">
+    <row r="37" spans="97:104" ht="18" x14ac:dyDescent="0.2">
       <c r="CZ37" s="19"/>
     </row>
-    <row r="51" spans="98:103">
+    <row r="51" spans="98:103" x14ac:dyDescent="0.2">
       <c r="CT51" s="18"/>
     </row>
-    <row r="53" spans="98:103">
+    <row r="53" spans="98:103" x14ac:dyDescent="0.2">
       <c r="CT53" s="20"/>
     </row>
-    <row r="60" spans="98:103">
+    <row r="60" spans="98:103" x14ac:dyDescent="0.2">
       <c r="CY60" s="21"/>
     </row>
-    <row r="70" spans="20:20">
+    <row r="70" spans="20:20" x14ac:dyDescent="0.2">
       <c r="T70" t="s">
         <v>0</v>
       </c>
@@ -21682,30 +21759,25 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG337"/>
+  <dimension ref="A1:AG339"/>
   <sheetViews>
     <sheetView zoomScale="117" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T339" sqref="T339"/>
+      <selection pane="bottomLeft" activeCell="T336" sqref="T336"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="37" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="37" customWidth="1"/>
     <col min="2" max="3" width="8" style="38" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="38" customWidth="1"/>
-    <col min="5" max="6" width="9.42578125" style="38" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="38" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="38" customWidth="1"/>
+    <col min="5" max="6" width="9.5" style="38" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="38" customWidth="1"/>
     <col min="8" max="8" width="8" style="38" customWidth="1"/>
     <col min="9" max="11" width="8" style="39" customWidth="1"/>
     <col min="12" max="19" width="8" style="39" hidden="1" customWidth="1"/>
@@ -21717,12 +21789,12 @@
     <col min="25" max="29" width="8" style="43" hidden="1" customWidth="1"/>
     <col min="30" max="31" width="8" style="108" hidden="1" customWidth="1"/>
     <col min="32" max="32" width="8" style="109" customWidth="1"/>
-    <col min="33" max="33" width="8.85546875" style="110" customWidth="1"/>
+    <col min="33" max="33" width="8.83203125" style="110" customWidth="1"/>
     <col min="34" max="34" width="10" style="43" customWidth="1"/>
     <col min="35" max="16384" width="8" style="43"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="35" customFormat="1" ht="105.75" customHeight="1">
+    <row r="1" spans="1:33" s="35" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="29" t="s">
         <v>1</v>
       </c>
@@ -21813,7 +21885,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="15">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A2" s="37">
         <v>44165</v>
       </c>
@@ -21863,7 +21935,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="15">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" s="37">
         <v>44166</v>
       </c>
@@ -21913,7 +21985,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="15">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" s="37">
         <v>44167</v>
       </c>
@@ -21963,7 +22035,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="15">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" s="37">
         <v>44168</v>
       </c>
@@ -22013,7 +22085,7 @@
         <v>9.5652173913043412E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="15">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" s="37">
         <v>44169</v>
       </c>
@@ -22063,7 +22135,7 @@
         <v>-0.24427480916030531</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="15">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7" s="37">
         <v>44172</v>
       </c>
@@ -22113,7 +22185,7 @@
         <v>-0.21311475409836061</v>
       </c>
     </row>
-    <row r="8" spans="1:33" ht="15">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8" s="37">
         <v>44173</v>
       </c>
@@ -22163,7 +22235,7 @@
         <v>-0.15887850467289713</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="15">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A9" s="37">
         <v>44174</v>
       </c>
@@ -22213,7 +22285,7 @@
         <v>-5.263157894736846E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:33" ht="15">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" s="37">
         <v>44175</v>
       </c>
@@ -22263,7 +22335,7 @@
         <v>-8.6956521739130474E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:33" ht="15">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A11" s="37">
         <v>44176</v>
       </c>
@@ -22313,7 +22385,7 @@
         <v>-0.35227272727272724</v>
       </c>
     </row>
-    <row r="12" spans="1:33" ht="15">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A12" s="37">
         <v>44179</v>
       </c>
@@ -22363,7 +22435,7 @@
         <v>0.71428571428571419</v>
       </c>
     </row>
-    <row r="13" spans="1:33" ht="15">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A13" s="37">
         <v>44180</v>
       </c>
@@ -22413,7 +22485,7 @@
         <v>-4.3956043956043918E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:33" ht="15">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A14" s="37">
         <v>44181</v>
       </c>
@@ -22463,7 +22535,7 @@
         <v>-0.28260869565217395</v>
       </c>
     </row>
-    <row r="15" spans="1:33" ht="15">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A15" s="37">
         <v>44182</v>
       </c>
@@ -22513,7 +22585,7 @@
         <v>0.42105263157894729</v>
       </c>
     </row>
-    <row r="16" spans="1:33" ht="15">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A16" s="37">
         <v>44183</v>
       </c>
@@ -22563,7 +22635,7 @@
         <v>0.15625</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="15">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A17" s="37">
         <v>44186</v>
       </c>
@@ -22613,7 +22685,7 @@
         <v>0.4423076923076924</v>
       </c>
     </row>
-    <row r="18" spans="1:33" ht="15">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A18" s="37">
         <v>44187</v>
       </c>
@@ -22663,7 +22735,7 @@
         <v>-0.25</v>
       </c>
     </row>
-    <row r="19" spans="1:33" ht="15">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A19" s="37">
         <v>44188</v>
       </c>
@@ -22713,7 +22785,7 @@
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:33" ht="15">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A20" s="37">
         <v>44189</v>
       </c>
@@ -22763,7 +22835,7 @@
         <v>-0.19402985074626861</v>
       </c>
     </row>
-    <row r="21" spans="1:33" ht="15">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A21" s="37">
         <v>44190</v>
       </c>
@@ -22813,7 +22885,7 @@
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:33" ht="15">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A22" s="37">
         <v>44193</v>
       </c>
@@ -22863,7 +22935,7 @@
         <v>0.15384615384615385</v>
       </c>
     </row>
-    <row r="23" spans="1:33" ht="15">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A23" s="37">
         <v>44194</v>
       </c>
@@ -22913,7 +22985,7 @@
         <v>3.6363636363636362E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:33" ht="15">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A24" s="37">
         <v>44195</v>
       </c>
@@ -22963,7 +23035,7 @@
         <v>3.2258064516129031E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:33" ht="15">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A25" s="37">
         <v>44196</v>
       </c>
@@ -23013,7 +23085,7 @@
         <v>-5.5248618784530426E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:33" ht="15">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A26" s="37">
         <v>44200</v>
       </c>
@@ -23063,7 +23135,7 @@
         <v>0.8033707865168539</v>
       </c>
     </row>
-    <row r="27" spans="1:33" ht="15">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A27" s="37">
         <v>44201</v>
       </c>
@@ -23113,7 +23185,7 @@
         <v>1.3157894736842105E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:33" ht="15">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A28" s="37">
         <v>44202</v>
       </c>
@@ -23163,7 +23235,7 @@
         <v>-0.42738589211618255</v>
       </c>
     </row>
-    <row r="29" spans="1:33" ht="15">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A29" s="37">
         <v>44203</v>
       </c>
@@ -23213,7 +23285,7 @@
         <v>-0.58260869565217399</v>
       </c>
     </row>
-    <row r="30" spans="1:33" ht="15">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A30" s="37">
         <v>44204</v>
       </c>
@@ -23263,7 +23335,7 @@
         <v>-5.161290322580641E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:33" ht="15">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A31" s="37">
         <v>44207</v>
       </c>
@@ -23313,7 +23385,7 @@
         <v>-5.5118110236220527E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:33" ht="15">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A32" s="37">
         <v>44208</v>
       </c>
@@ -23363,7 +23435,7 @@
         <v>0.73553719008264451</v>
       </c>
     </row>
-    <row r="33" spans="1:33" ht="15">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A33" s="37">
         <v>44209</v>
       </c>
@@ -23413,7 +23485,7 @@
         <v>-0.26415094339622641</v>
       </c>
     </row>
-    <row r="34" spans="1:33" ht="15">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A34" s="37">
         <v>44210</v>
       </c>
@@ -23463,7 +23535,7 @@
         <v>0.389261744966443</v>
       </c>
     </row>
-    <row r="35" spans="1:33" ht="15">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A35" s="37">
         <v>44211</v>
       </c>
@@ -23513,7 +23585,7 @@
         <v>0.31460674157303364</v>
       </c>
     </row>
-    <row r="36" spans="1:33" ht="15">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A36" s="37">
         <v>44214</v>
       </c>
@@ -23563,7 +23635,7 @@
         <v>0.43548387096774194</v>
       </c>
     </row>
-    <row r="37" spans="1:33" ht="15">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A37" s="37">
         <v>44215</v>
       </c>
@@ -23613,7 +23685,7 @@
         <v>-7.2033898305084804E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:33" ht="15">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A38" s="37">
         <v>44216</v>
       </c>
@@ -23663,7 +23735,7 @@
         <v>-6.25E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:33" ht="15">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A39" s="37">
         <v>44217</v>
       </c>
@@ -23713,7 +23785,7 @@
         <v>-1.2658227848101266E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:33" ht="15">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A40" s="37">
         <v>44218</v>
       </c>
@@ -23763,7 +23835,7 @@
         <v>-0.34955752212389374</v>
       </c>
     </row>
-    <row r="41" spans="1:33" ht="15">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A41" s="37">
         <v>44221</v>
       </c>
@@ -23813,7 +23885,7 @@
         <v>-0.31683168316831678</v>
       </c>
     </row>
-    <row r="42" spans="1:33" ht="15">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A42" s="37">
         <v>44222</v>
       </c>
@@ -23863,7 +23935,7 @@
         <v>-0.11560693641618494</v>
       </c>
     </row>
-    <row r="43" spans="1:33" ht="15">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A43" s="37">
         <v>44223</v>
       </c>
@@ -23913,7 +23985,7 @@
         <v>0.27397260273972607</v>
       </c>
     </row>
-    <row r="44" spans="1:33" ht="15">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A44" s="37">
         <v>44224</v>
       </c>
@@ -23963,7 +24035,7 @@
         <v>-0.20754716981132076</v>
       </c>
     </row>
-    <row r="45" spans="1:33" ht="15">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A45" s="37">
         <v>44225</v>
       </c>
@@ -24013,7 +24085,7 @@
         <v>-0.38064516129032255</v>
       </c>
     </row>
-    <row r="46" spans="1:33" ht="15">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A46" s="37">
         <v>44228</v>
       </c>
@@ -24063,7 +24135,7 @@
         <v>0.80882352941176461</v>
       </c>
     </row>
-    <row r="47" spans="1:33" ht="15">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A47" s="37">
         <v>44229</v>
       </c>
@@ -24113,7 +24185,7 @@
         <v>0.30769230769230771</v>
       </c>
     </row>
-    <row r="48" spans="1:33" ht="15">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A48" s="37">
         <v>44230</v>
       </c>
@@ -24163,7 +24235,7 @@
         <v>-0.3571428571428571</v>
       </c>
     </row>
-    <row r="49" spans="1:33" ht="15">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A49" s="37">
         <v>44231</v>
       </c>
@@ -24213,7 +24285,7 @@
         <v>-0.2857142857142857</v>
       </c>
     </row>
-    <row r="50" spans="1:33" ht="15">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A50" s="37">
         <v>44232</v>
       </c>
@@ -24263,7 +24335,7 @@
         <v>-0.11184210526315785</v>
       </c>
     </row>
-    <row r="51" spans="1:33" ht="15">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A51" s="37">
         <v>44235</v>
       </c>
@@ -24313,7 +24385,7 @@
         <v>0.27906976744186046</v>
       </c>
     </row>
-    <row r="52" spans="1:33" ht="15">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A52" s="37">
         <v>44236</v>
       </c>
@@ -24363,7 +24435,7 @@
         <v>0.34482758620689646</v>
       </c>
     </row>
-    <row r="53" spans="1:33" ht="15">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A53" s="37">
         <v>44237</v>
       </c>
@@ -24413,7 +24485,7 @@
         <v>-0.29090909090909089</v>
       </c>
     </row>
-    <row r="54" spans="1:33" ht="15">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A54" s="37">
         <v>44245</v>
       </c>
@@ -24463,7 +24535,7 @@
         <v>0.8867924528301887</v>
       </c>
     </row>
-    <row r="55" spans="1:33" ht="15">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A55" s="37">
         <v>44246</v>
       </c>
@@ -24513,7 +24585,7 @@
         <v>0.47058823529411764</v>
       </c>
     </row>
-    <row r="56" spans="1:33" ht="15">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A56" s="37">
         <v>44249</v>
       </c>
@@ -24563,7 +24635,7 @@
         <v>4.1841004184099825E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:33" ht="15">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A57" s="37">
         <v>44250</v>
       </c>
@@ -24613,7 +24685,7 @@
         <v>-0.43214285714285711</v>
       </c>
     </row>
-    <row r="58" spans="1:33" ht="15">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A58" s="37">
         <v>44251</v>
       </c>
@@ -24663,7 +24735,7 @@
         <v>-0.45922746781115881</v>
       </c>
     </row>
-    <row r="59" spans="1:33" ht="15">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A59" s="37">
         <v>44252</v>
       </c>
@@ -24713,7 +24785,7 @@
         <v>-0.29714285714285715</v>
       </c>
     </row>
-    <row r="60" spans="1:33" ht="15">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A60" s="37">
         <v>44253</v>
       </c>
@@ -24763,7 +24835,7 @@
         <v>-0.13970588235294124</v>
       </c>
     </row>
-    <row r="61" spans="1:33" ht="15">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A61" s="44">
         <v>44256</v>
       </c>
@@ -24831,7 +24903,7 @@
         <v>1.0655737704918034</v>
       </c>
     </row>
-    <row r="62" spans="1:33" ht="15">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A62" s="51">
         <v>44257</v>
       </c>
@@ -24899,7 +24971,7 @@
         <v>-0.32317073170731703</v>
       </c>
     </row>
-    <row r="63" spans="1:33" ht="15">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A63" s="37">
         <v>44258</v>
       </c>
@@ -24949,7 +25021,7 @@
         <v>0.51874999999999993</v>
       </c>
     </row>
-    <row r="64" spans="1:33" ht="15">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A64" s="37">
         <v>44259</v>
       </c>
@@ -24999,7 +25071,7 @@
         <v>-0.37623762376237618</v>
       </c>
     </row>
-    <row r="65" spans="1:33" ht="15">
+    <row r="65" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A65" s="37">
         <v>44260</v>
       </c>
@@ -25049,7 +25121,7 @@
         <v>0.14374999999999996</v>
       </c>
     </row>
-    <row r="66" spans="1:33" ht="15">
+    <row r="66" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A66" s="37">
         <v>44263</v>
       </c>
@@ -25099,7 +25171,7 @@
         <v>-0.13586956521739132</v>
       </c>
     </row>
-    <row r="67" spans="1:33" ht="15">
+    <row r="67" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A67" s="37">
         <v>44264</v>
       </c>
@@ -25149,7 +25221,7 @@
         <v>-0.34615384615384615</v>
       </c>
     </row>
-    <row r="68" spans="1:33" ht="15">
+    <row r="68" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A68" s="37">
         <v>44265</v>
       </c>
@@ -25199,7 +25271,7 @@
         <v>-0.33108108108108109</v>
       </c>
     </row>
-    <row r="69" spans="1:33" ht="15">
+    <row r="69" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A69" s="37">
         <v>44266</v>
       </c>
@@ -25249,7 +25321,7 @@
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="70" spans="1:33" ht="15">
+    <row r="70" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A70" s="37">
         <v>44267</v>
       </c>
@@ -25299,7 +25371,7 @@
         <v>3.6764705882352887E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:33" ht="15">
+    <row r="71" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A71" s="37">
         <v>44270</v>
       </c>
@@ -25349,7 +25421,7 @@
         <v>-7.3825503355704647E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:33" ht="15">
+    <row r="72" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A72" s="37">
         <v>44271</v>
       </c>
@@ -25399,7 +25471,7 @@
         <v>0.18518518518518517</v>
       </c>
     </row>
-    <row r="73" spans="1:33" ht="15">
+    <row r="73" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A73" s="37">
         <v>44272</v>
       </c>
@@ -25449,7 +25521,7 @@
         <v>7.006369426751588E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:33" ht="15">
+    <row r="74" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A74" s="37">
         <v>44273</v>
       </c>
@@ -25499,7 +25571,7 @@
         <v>6.6265060240963805E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:33" ht="15">
+    <row r="75" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A75" s="37">
         <v>44274</v>
       </c>
@@ -25549,7 +25621,7 @@
         <v>-9.4972067039106114E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:33" ht="15">
+    <row r="76" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A76" s="37">
         <v>44277</v>
       </c>
@@ -25599,7 +25671,7 @@
         <v>0.4201183431952662</v>
       </c>
     </row>
-    <row r="77" spans="1:33" ht="15">
+    <row r="77" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A77" s="37">
         <v>44278</v>
       </c>
@@ -25649,7 +25721,7 @@
         <v>-0.26943005181347146</v>
       </c>
     </row>
-    <row r="78" spans="1:33" ht="15">
+    <row r="78" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A78" s="37">
         <v>44279</v>
       </c>
@@ -25699,7 +25771,7 @@
         <v>-7.1823204419889541E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:33" ht="15">
+    <row r="79" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A79" s="37">
         <v>44280</v>
       </c>
@@ -25749,7 +25821,7 @@
         <v>-0.29508196721311475</v>
       </c>
     </row>
-    <row r="80" spans="1:33" ht="15">
+    <row r="80" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A80" s="37">
         <v>44281</v>
       </c>
@@ -25799,7 +25871,7 @@
         <v>0.47945205479452063</v>
       </c>
     </row>
-    <row r="81" spans="1:33" ht="15">
+    <row r="81" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A81" s="37">
         <v>44284</v>
       </c>
@@ -25849,7 +25921,7 @@
         <v>0.12280701754385964</v>
       </c>
     </row>
-    <row r="82" spans="1:33" ht="15">
+    <row r="82" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A82" s="37">
         <v>44285</v>
       </c>
@@ -25899,7 +25971,7 @@
         <v>-2.7932960893854709E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:33" ht="15">
+    <row r="83" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A83" s="37">
         <v>44286</v>
       </c>
@@ -25949,7 +26021,7 @@
         <v>0.12886597938144323</v>
       </c>
     </row>
-    <row r="84" spans="1:33" ht="15">
+    <row r="84" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A84" s="37">
         <v>44287</v>
       </c>
@@ -25999,7 +26071,7 @@
         <v>0.1076923076923077</v>
       </c>
     </row>
-    <row r="85" spans="1:33" ht="15">
+    <row r="85" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A85" s="37">
         <v>44288</v>
       </c>
@@ -26049,7 +26121,7 @@
         <v>4.9261083743841663E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:33" ht="15">
+    <row r="86" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A86" s="37">
         <v>44292</v>
       </c>
@@ -26100,7 +26172,7 @@
         <v>7.0422535211267609E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:33" ht="15">
+    <row r="87" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A87" s="37">
         <v>44293</v>
       </c>
@@ -26151,7 +26223,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="88" spans="1:33" ht="15">
+    <row r="88" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A88" s="58">
         <v>44294</v>
       </c>
@@ -26220,7 +26292,7 @@
         <v>-0.52564102564102566</v>
       </c>
     </row>
-    <row r="89" spans="1:33" ht="15">
+    <row r="89" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A89" s="37">
         <v>44295</v>
       </c>
@@ -26271,7 +26343,7 @@
         <v>-0.18719211822660103</v>
       </c>
     </row>
-    <row r="90" spans="1:33" ht="15">
+    <row r="90" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A90" s="37">
         <v>44298</v>
       </c>
@@ -26322,7 +26394,7 @@
         <v>5.4945054945054986E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:33" ht="15">
+    <row r="91" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A91" s="37">
         <v>44299</v>
       </c>
@@ -26373,7 +26445,7 @@
         <v>-1.9230769230769232E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:33" ht="15">
+    <row r="92" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A92" s="37">
         <v>44300</v>
       </c>
@@ -26423,7 +26495,7 @@
         <v>0.12941176470588239</v>
       </c>
     </row>
-    <row r="93" spans="1:33" ht="15">
+    <row r="93" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A93" s="58">
         <v>44301</v>
       </c>
@@ -26491,7 +26563,7 @@
         <v>-0.27932960893854747</v>
       </c>
     </row>
-    <row r="94" spans="1:33" ht="15">
+    <row r="94" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A94" s="37">
         <v>44302</v>
       </c>
@@ -26541,7 +26613,7 @@
         <v>0.40506329113924056</v>
       </c>
     </row>
-    <row r="95" spans="1:33" ht="15">
+    <row r="95" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A95" s="37">
         <v>44305</v>
       </c>
@@ -26591,7 +26663,7 @@
         <v>0.27624309392265189</v>
       </c>
     </row>
-    <row r="96" spans="1:33" ht="15">
+    <row r="96" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A96" s="37">
         <v>44306</v>
       </c>
@@ -26641,7 +26713,7 @@
         <v>-0.365979381443299</v>
       </c>
     </row>
-    <row r="97" spans="1:33" ht="15">
+    <row r="97" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A97" s="37">
         <v>44307</v>
       </c>
@@ -26691,7 +26763,7 @@
         <v>-0.46875</v>
       </c>
     </row>
-    <row r="98" spans="1:33" ht="15">
+    <row r="98" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A98" s="37">
         <v>44308</v>
       </c>
@@ -26741,7 +26813,7 @@
         <v>-0.21052631578947364</v>
       </c>
     </row>
-    <row r="99" spans="1:33" ht="15">
+    <row r="99" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A99" s="37">
         <v>44309</v>
       </c>
@@ -26791,7 +26863,7 @@
         <v>-8.6956521739130488E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:33" ht="15">
+    <row r="100" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A100" s="37">
         <v>44312</v>
       </c>
@@ -26841,7 +26913,7 @@
         <v>0.26605504587155954</v>
       </c>
     </row>
-    <row r="101" spans="1:33" ht="15">
+    <row r="101" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A101" s="65">
         <v>44313</v>
       </c>
@@ -26909,7 +26981,7 @@
         <v>-5.7851239669421545E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:33" ht="15">
+    <row r="102" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A102" s="37">
         <v>44314</v>
       </c>
@@ -26959,7 +27031,7 @@
         <v>0.51260504201680679</v>
       </c>
     </row>
-    <row r="103" spans="1:33" ht="15">
+    <row r="103" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A103" s="37">
         <v>44315</v>
       </c>
@@ -27009,7 +27081,7 @@
         <v>-8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:33" ht="15">
+    <row r="104" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A104" s="37">
         <v>44316</v>
       </c>
@@ -27059,7 +27131,7 @@
         <v>-0.15492957746478878</v>
       </c>
     </row>
-    <row r="105" spans="1:33" ht="15">
+    <row r="105" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A105" s="37">
         <v>44322</v>
       </c>
@@ -27109,7 +27181,7 @@
         <v>0.20833333333333334</v>
       </c>
     </row>
-    <row r="106" spans="1:33" ht="15">
+    <row r="106" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A106" s="37">
         <v>44323</v>
       </c>
@@ -27159,7 +27231,7 @@
         <v>-9.1549295774647932E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:33" ht="15">
+    <row r="107" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A107" s="72">
         <v>44326</v>
       </c>
@@ -27227,7 +27299,7 @@
         <v>0.74468085106382975</v>
       </c>
     </row>
-    <row r="108" spans="1:33" ht="15">
+    <row r="108" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A108" s="37">
         <v>44327</v>
       </c>
@@ -27277,7 +27349,7 @@
         <v>-0.11475409836065574</v>
       </c>
     </row>
-    <row r="109" spans="1:33" ht="15">
+    <row r="109" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A109" s="37">
         <v>44328</v>
       </c>
@@ -27327,7 +27399,7 @@
         <v>-0.2960893854748603</v>
       </c>
     </row>
-    <row r="110" spans="1:33" ht="15">
+    <row r="110" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A110" s="37">
         <v>44329</v>
       </c>
@@ -27377,7 +27449,7 @@
         <v>0.297752808988764</v>
       </c>
     </row>
-    <row r="111" spans="1:33" ht="15">
+    <row r="111" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A111" s="58">
         <v>44333</v>
       </c>
@@ -27445,7 +27517,7 @@
         <v>-0.44508670520231214</v>
       </c>
     </row>
-    <row r="112" spans="1:33" ht="15">
+    <row r="112" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A112" s="37">
         <v>44334</v>
       </c>
@@ -27495,7 +27567,7 @@
         <v>0.37086092715231783</v>
       </c>
     </row>
-    <row r="113" spans="1:33" ht="15">
+    <row r="113" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A113" s="37">
         <v>44335</v>
       </c>
@@ -27545,7 +27617,7 @@
         <v>-0.1067415730337079</v>
       </c>
     </row>
-    <row r="114" spans="1:33" ht="15">
+    <row r="114" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A114" s="37">
         <v>44336</v>
       </c>
@@ -27595,7 +27667,7 @@
         <v>-0.10389610389610393</v>
       </c>
     </row>
-    <row r="115" spans="1:33" ht="15">
+    <row r="115" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A115" s="37">
         <v>44337</v>
       </c>
@@ -27645,7 +27717,7 @@
         <v>0.10714285714285714</v>
       </c>
     </row>
-    <row r="116" spans="1:33" ht="15">
+    <row r="116" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A116" s="37">
         <v>44340</v>
       </c>
@@ -27695,7 +27767,7 @@
         <v>4.3478260869565265E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:33" ht="15">
+    <row r="117" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A117" s="37">
         <v>44341</v>
       </c>
@@ -27745,7 +27817,7 @@
         <v>-0.12195121951219508</v>
       </c>
     </row>
-    <row r="118" spans="1:33" ht="15">
+    <row r="118" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A118" s="37">
         <v>44342</v>
       </c>
@@ -27795,7 +27867,7 @@
         <v>6.6265060240963805E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:33" ht="15">
+    <row r="119" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A119" s="37">
         <v>44343</v>
       </c>
@@ -27845,7 +27917,7 @@
         <v>0.19631901840490792</v>
       </c>
     </row>
-    <row r="120" spans="1:33" ht="15">
+    <row r="120" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A120" s="37">
         <v>44344</v>
       </c>
@@ -27895,7 +27967,7 @@
         <v>-0.16279069767441864</v>
       </c>
     </row>
-    <row r="121" spans="1:33" ht="15">
+    <row r="121" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A121" s="37">
         <v>44347</v>
       </c>
@@ -27945,7 +28017,7 @@
         <v>0.48255813953488363</v>
       </c>
     </row>
-    <row r="122" spans="1:33" ht="15">
+    <row r="122" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A122" s="37">
         <v>44348</v>
       </c>
@@ -27999,7 +28071,7 @@
         <v>1.5151515151515152E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:33" ht="15">
+    <row r="123" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A123" s="65">
         <v>44349</v>
       </c>
@@ -28067,7 +28139,7 @@
         <v>-0.19000000000000006</v>
       </c>
     </row>
-    <row r="124" spans="1:33" ht="15">
+    <row r="124" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A124" s="37">
         <v>44350</v>
       </c>
@@ -28117,7 +28189,7 @@
         <v>-8.2524271844660255E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:33" ht="15">
+    <row r="125" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A125" s="37">
         <v>44351</v>
       </c>
@@ -28167,7 +28239,7 @@
         <v>-0.20108695652173916</v>
       </c>
     </row>
-    <row r="126" spans="1:33" ht="15">
+    <row r="126" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A126" s="37">
         <v>44354</v>
       </c>
@@ -28217,7 +28289,7 @@
         <v>8.4337349397590314E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:33" ht="15">
+    <row r="127" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A127" s="37">
         <v>44355</v>
       </c>
@@ -28267,7 +28339,7 @@
         <v>-7.5581395348837246E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:33" ht="15">
+    <row r="128" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A128" s="37">
         <v>44356</v>
       </c>
@@ -28317,7 +28389,7 @@
         <v>-5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:33" ht="15">
+    <row r="129" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A129" s="37">
         <v>44357</v>
       </c>
@@ -28367,7 +28439,7 @@
         <v>0.15243902439024395</v>
       </c>
     </row>
-    <row r="130" spans="1:33" ht="15">
+    <row r="130" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A130" s="37">
         <v>44358</v>
       </c>
@@ -28417,7 +28489,7 @@
         <v>7.7844311377245554E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:33" ht="15">
+    <row r="131" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A131" s="65">
         <v>44362</v>
       </c>
@@ -28485,7 +28557,7 @@
         <v>-0.34482758620689657</v>
       </c>
     </row>
-    <row r="132" spans="1:33" ht="15">
+    <row r="132" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A132" s="65">
         <v>44363</v>
       </c>
@@ -28535,7 +28607,7 @@
         <v>-0.34782608695652173</v>
       </c>
     </row>
-    <row r="133" spans="1:33" ht="15">
+    <row r="133" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A133" s="37">
         <v>44364</v>
       </c>
@@ -28585,7 +28657,7 @@
         <v>0.10526315789473678</v>
       </c>
     </row>
-    <row r="134" spans="1:33" ht="15">
+    <row r="134" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A134" s="37">
         <v>44365</v>
       </c>
@@ -28635,7 +28707,7 @@
         <v>0.4262295081967214</v>
       </c>
     </row>
-    <row r="135" spans="1:33" ht="15">
+    <row r="135" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A135" s="37">
         <v>44368</v>
       </c>
@@ -28685,7 +28757,7 @@
         <v>0.45774647887323938</v>
       </c>
     </row>
-    <row r="136" spans="1:33" ht="15">
+    <row r="136" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A136" s="37">
         <v>44369</v>
       </c>
@@ -28735,7 +28807,7 @@
         <v>0.12500000000000006</v>
       </c>
     </row>
-    <row r="137" spans="1:33" ht="15">
+    <row r="137" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A137" s="37">
         <v>44370</v>
       </c>
@@ -28785,7 +28857,7 @@
         <v>-0.20725388601036263</v>
       </c>
     </row>
-    <row r="138" spans="1:33" ht="15">
+    <row r="138" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A138" s="37">
         <v>44371</v>
       </c>
@@ -28835,7 +28907,7 @@
         <v>-0.11290322580645161</v>
       </c>
     </row>
-    <row r="139" spans="1:33" ht="15">
+    <row r="139" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A139" s="37">
         <v>44372</v>
       </c>
@@ -28885,7 +28957,7 @@
         <v>-2.3255813953488413E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:33" ht="15">
+    <row r="140" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A140" s="37">
         <v>44375</v>
       </c>
@@ -28935,7 +29007,7 @@
         <v>0.14814814814814814</v>
       </c>
     </row>
-    <row r="141" spans="1:33" ht="15">
+    <row r="141" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A141" s="37">
         <v>44376</v>
       </c>
@@ -28985,7 +29057,7 @@
         <v>-0.25433526011560692</v>
       </c>
     </row>
-    <row r="142" spans="1:33" ht="15">
+    <row r="142" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A142" s="37">
         <v>44377</v>
       </c>
@@ -29035,7 +29107,7 @@
         <v>-4.9689440993788775E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:33" ht="15">
+    <row r="143" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A143" s="37">
         <v>44378</v>
       </c>
@@ -29085,7 +29157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:33" ht="15">
+    <row r="144" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A144" s="37">
         <v>44379</v>
       </c>
@@ -29135,7 +29207,7 @@
         <v>-0.26027397260273971</v>
       </c>
     </row>
-    <row r="145" spans="1:33" ht="15">
+    <row r="145" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A145" s="37">
         <v>44382</v>
       </c>
@@ -29185,7 +29257,7 @@
         <v>0.51079136690647475</v>
       </c>
     </row>
-    <row r="146" spans="1:33" ht="15">
+    <row r="146" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A146" s="37">
         <v>44383</v>
       </c>
@@ -29235,7 +29307,7 @@
         <v>-0.27848101265822783</v>
       </c>
     </row>
-    <row r="147" spans="1:33" ht="15">
+    <row r="147" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A147" s="37">
         <v>44384</v>
       </c>
@@ -29285,7 +29357,7 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="148" spans="1:33" ht="15">
+    <row r="148" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A148" s="37">
         <v>44385</v>
       </c>
@@ -29335,7 +29407,7 @@
         <v>-0.19298245614035087</v>
       </c>
     </row>
-    <row r="149" spans="1:33" ht="15">
+    <row r="149" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A149" s="37">
         <v>44386</v>
       </c>
@@ -29385,7 +29457,7 @@
         <v>0.30612244897959184</v>
       </c>
     </row>
-    <row r="150" spans="1:33" ht="15">
+    <row r="150" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A150" s="37">
         <v>44389</v>
       </c>
@@ -29435,7 +29507,7 @@
         <v>0.43930635838150295</v>
       </c>
     </row>
-    <row r="151" spans="1:33" ht="15">
+    <row r="151" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A151" s="37">
         <v>44390</v>
       </c>
@@ -29485,7 +29557,7 @@
         <v>-2.0725388601036197E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:33" ht="15">
+    <row r="152" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A152" s="37">
         <v>44391</v>
       </c>
@@ -29535,7 +29607,7 @@
         <v>-0.25714285714285712</v>
       </c>
     </row>
-    <row r="153" spans="1:33" ht="15">
+    <row r="153" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A153" s="37">
         <v>44392</v>
       </c>
@@ -29585,7 +29657,7 @@
         <v>-0.31818181818181818</v>
       </c>
     </row>
-    <row r="154" spans="1:33" ht="15">
+    <row r="154" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A154" s="37">
         <v>44393</v>
       </c>
@@ -29635,7 +29707,7 @@
         <v>-0.34375000000000006</v>
       </c>
     </row>
-    <row r="155" spans="1:33" ht="15">
+    <row r="155" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A155" s="37">
         <v>44396</v>
       </c>
@@ -29685,7 +29757,7 @@
         <v>0.18181818181818182</v>
       </c>
     </row>
-    <row r="156" spans="1:33" ht="15">
+    <row r="156" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A156" s="37">
         <v>44397</v>
       </c>
@@ -29735,7 +29807,7 @@
         <v>4.5454545454545456E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:33" ht="15">
+    <row r="157" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A157" s="37">
         <v>44398</v>
       </c>
@@ -29785,7 +29857,7 @@
         <v>0.89473684210526305</v>
       </c>
     </row>
-    <row r="158" spans="1:33" ht="15">
+    <row r="158" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A158" s="37">
         <v>44399</v>
       </c>
@@ -29835,7 +29907,7 @@
         <v>-7.6923076923076886E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:33" ht="15">
+    <row r="159" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A159" s="37">
         <v>44400</v>
       </c>
@@ -29885,7 +29957,7 @@
         <v>-0.24193548387096775</v>
       </c>
     </row>
-    <row r="160" spans="1:33" ht="15">
+    <row r="160" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A160" s="37">
         <v>44403</v>
       </c>
@@ -29935,7 +30007,7 @@
         <v>-0.40641711229946526</v>
       </c>
     </row>
-    <row r="161" spans="1:33" ht="15">
+    <row r="161" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A161" s="37">
         <v>44404</v>
       </c>
@@ -29985,7 +30057,7 @@
         <v>-0.44285714285714284</v>
       </c>
     </row>
-    <row r="162" spans="1:33" ht="15">
+    <row r="162" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A162" s="37">
         <v>44405</v>
       </c>
@@ -30035,7 +30107,7 @@
         <v>9.0909090909091564E-3</v>
       </c>
     </row>
-    <row r="163" spans="1:33" ht="15">
+    <row r="163" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A163" s="37">
         <v>44406</v>
       </c>
@@ -30085,7 +30157,7 @@
         <v>2.4499999999999997</v>
       </c>
     </row>
-    <row r="164" spans="1:33" ht="15">
+    <row r="164" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A164" s="37">
         <v>44407</v>
       </c>
@@ -30135,7 +30207,7 @@
         <v>0.36516853932584264</v>
       </c>
     </row>
-    <row r="165" spans="1:33" ht="15">
+    <row r="165" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A165" s="37">
         <v>44410</v>
       </c>
@@ -30185,7 +30257,7 @@
         <v>0.23605150214592266</v>
       </c>
     </row>
-    <row r="166" spans="1:33" ht="15">
+    <row r="166" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A166" s="37">
         <v>44411</v>
       </c>
@@ -30235,7 +30307,7 @@
         <v>-0.45547945205479451</v>
       </c>
     </row>
-    <row r="167" spans="1:33" ht="15">
+    <row r="167" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A167" s="37">
         <v>44412</v>
       </c>
@@ -30285,7 +30357,7 @@
         <v>0.13478260869565212</v>
       </c>
     </row>
-    <row r="168" spans="1:33" ht="15">
+    <row r="168" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A168" s="37">
         <v>44413</v>
       </c>
@@ -30335,7 +30407,7 @@
         <v>-0.36440677966101698</v>
       </c>
     </row>
-    <row r="169" spans="1:33" ht="15">
+    <row r="169" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A169" s="37">
         <v>44414</v>
       </c>
@@ -30385,7 +30457,7 @@
         <v>-6.842105263157898E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:33" ht="15">
+    <row r="170" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A170" s="37">
         <v>44417</v>
       </c>
@@ -30435,7 +30507,7 @@
         <v>0.20918367346938785</v>
       </c>
     </row>
-    <row r="171" spans="1:33" ht="15">
+    <row r="171" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A171" s="37">
         <v>44418</v>
       </c>
@@ -30485,7 +30557,7 @@
         <v>0.11702127659574472</v>
       </c>
     </row>
-    <row r="172" spans="1:33" ht="15">
+    <row r="172" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A172" s="37">
         <v>44419</v>
       </c>
@@ -30535,7 +30607,7 @@
         <v>0.29807692307692318</v>
       </c>
     </row>
-    <row r="173" spans="1:33" ht="15">
+    <row r="173" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A173" s="37">
         <v>44420</v>
       </c>
@@ -30585,7 +30657,7 @@
         <v>-0.17154811715481177</v>
       </c>
     </row>
-    <row r="174" spans="1:33" ht="15">
+    <row r="174" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A174" s="37">
         <v>44423</v>
       </c>
@@ -30635,7 +30707,7 @@
         <v>-0.13716814159292029</v>
       </c>
     </row>
-    <row r="175" spans="1:33" ht="15">
+    <row r="175" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A175" s="37">
         <v>44424</v>
       </c>
@@ -30685,7 +30757,7 @@
         <v>-3.6199095022624493E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:33" ht="15">
+    <row r="176" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A176" s="37">
         <v>44425</v>
       </c>
@@ -30735,7 +30807,7 @@
         <v>-0.59900990099009899</v>
       </c>
     </row>
-    <row r="177" spans="1:33" ht="15">
+    <row r="177" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A177" s="37">
         <v>44426</v>
       </c>
@@ -30785,7 +30857,7 @@
         <v>0.26993865030674841</v>
       </c>
     </row>
-    <row r="178" spans="1:33" ht="15">
+    <row r="178" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A178" s="37">
         <v>44427</v>
       </c>
@@ -30843,7 +30915,7 @@
         <v>-0.1736526946107784</v>
       </c>
     </row>
-    <row r="179" spans="1:33" ht="15">
+    <row r="179" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A179" s="87">
         <v>44428</v>
       </c>
@@ -30911,7 +30983,7 @@
         <v>-2.8169014084507091E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:33" ht="15">
+    <row r="180" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A180" s="37">
         <v>44431</v>
       </c>
@@ -30969,7 +31041,7 @@
         <v>1.2732919254658388</v>
       </c>
     </row>
-    <row r="181" spans="1:33" ht="15">
+    <row r="181" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A181" s="37">
         <v>44432</v>
       </c>
@@ -31027,7 +31099,7 @@
         <v>-7.4766355140186855E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:33" ht="15">
+    <row r="182" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A182" s="37">
         <v>44433</v>
       </c>
@@ -31077,7 +31149,7 @@
         <v>3.8461538461538464E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:33" ht="15">
+    <row r="183" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A183" s="37">
         <v>44434</v>
       </c>
@@ -31127,7 +31199,7 @@
         <v>-0.39776951672862459</v>
       </c>
     </row>
-    <row r="184" spans="1:33" ht="15">
+    <row r="184" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A184" s="37">
         <v>44435</v>
       </c>
@@ -31177,7 +31249,7 @@
         <v>8.9552238805970144E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:33" ht="15">
+    <row r="185" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A185" s="37">
         <v>44438</v>
       </c>
@@ -31227,7 +31299,7 @@
         <v>0.11057692307692316</v>
       </c>
     </row>
-    <row r="186" spans="1:33" ht="15">
+    <row r="186" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A186" s="37">
         <v>44439</v>
       </c>
@@ -31277,7 +31349,7 @@
         <v>0.16176470588235295</v>
       </c>
     </row>
-    <row r="187" spans="1:33" ht="15">
+    <row r="187" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A187" s="37">
         <v>44440</v>
       </c>
@@ -31327,7 +31399,7 @@
         <v>-0.14847161572052398</v>
       </c>
     </row>
-    <row r="188" spans="1:33" ht="15">
+    <row r="188" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A188" s="37">
         <v>44441</v>
       </c>
@@ -31377,7 +31449,7 @@
         <v>0.47963800904977366</v>
       </c>
     </row>
-    <row r="189" spans="1:33" ht="15">
+    <row r="189" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A189" s="37">
         <v>44442</v>
       </c>
@@ -31427,7 +31499,7 @@
         <v>-0.38339920948616596</v>
       </c>
     </row>
-    <row r="190" spans="1:33" ht="15">
+    <row r="190" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A190" s="37">
         <v>44445</v>
       </c>
@@ -31477,7 +31549,7 @@
         <v>4.8672566371681485E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:33" ht="15">
+    <row r="191" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A191" s="37">
         <v>44446</v>
       </c>
@@ -31527,7 +31599,7 @@
         <v>0.1875</v>
       </c>
     </row>
-    <row r="192" spans="1:33" ht="15">
+    <row r="192" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A192" s="37">
         <v>44447</v>
       </c>
@@ -31577,7 +31649,7 @@
         <v>0.18141592920353991</v>
       </c>
     </row>
-    <row r="193" spans="1:33" ht="15">
+    <row r="193" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A193" s="37">
         <v>44448</v>
       </c>
@@ -31627,7 +31699,7 @@
         <v>-0.19011406844106468</v>
       </c>
     </row>
-    <row r="194" spans="1:33" ht="15">
+    <row r="194" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A194" s="37">
         <v>44449</v>
       </c>
@@ -31677,7 +31749,7 @@
         <v>-0.37647058823529411</v>
       </c>
     </row>
-    <row r="195" spans="1:33" ht="15">
+    <row r="195" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A195" s="37">
         <v>44452</v>
       </c>
@@ -31727,7 +31799,7 @@
         <v>0.19718309859154928</v>
       </c>
     </row>
-    <row r="196" spans="1:33" ht="15">
+    <row r="196" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A196" s="37">
         <v>44453</v>
       </c>
@@ -31777,7 +31849,7 @@
         <v>-9.5693779904306275E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:33" ht="15">
+    <row r="197" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A197" s="37">
         <v>44454</v>
       </c>
@@ -31835,7 +31907,7 @@
         <v>0.34328358208955223</v>
       </c>
     </row>
-    <row r="198" spans="1:33" ht="15">
+    <row r="198" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A198" s="87">
         <v>44455</v>
       </c>
@@ -31903,7 +31975,7 @@
         <v>-0.42016806722689071</v>
       </c>
     </row>
-    <row r="199" spans="1:33" ht="15">
+    <row r="199" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A199" s="87">
         <v>44456</v>
       </c>
@@ -31971,7 +32043,7 @@
         <v>-0.29145728643216073</v>
       </c>
     </row>
-    <row r="200" spans="1:33" ht="15">
+    <row r="200" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A200" s="37">
         <v>44461</v>
       </c>
@@ -32029,7 +32101,7 @@
         <v>0.57377049180327866</v>
       </c>
     </row>
-    <row r="201" spans="1:33" ht="15">
+    <row r="201" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A201" s="37">
         <v>44462</v>
       </c>
@@ -32087,7 +32159,7 @@
         <v>9.5238095238095233E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:33" ht="15">
+    <row r="202" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A202" s="37">
         <v>44463</v>
       </c>
@@ -32137,7 +32209,7 @@
         <v>-0.419811320754717</v>
       </c>
     </row>
-    <row r="203" spans="1:33" ht="15">
+    <row r="203" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A203" s="87">
         <v>44466</v>
       </c>
@@ -32188,7 +32260,7 @@
         <v>-0.41747572815533984</v>
       </c>
     </row>
-    <row r="204" spans="1:33" ht="15">
+    <row r="204" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A204" s="37">
         <v>44467</v>
       </c>
@@ -32238,7 +32310,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="205" spans="1:33" ht="15">
+    <row r="205" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A205" s="87">
         <v>44468</v>
       </c>
@@ -32289,7 +32361,7 @@
         <v>-0.64473684210526316</v>
       </c>
     </row>
-    <row r="206" spans="1:33" ht="15">
+    <row r="206" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A206" s="37">
         <v>44469</v>
       </c>
@@ -32339,7 +32411,7 @@
         <v>0.69767441860465118</v>
       </c>
     </row>
-    <row r="207" spans="1:33" ht="15">
+    <row r="207" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A207" s="37">
         <v>44477</v>
       </c>
@@ -32389,7 +32461,7 @@
         <v>0.18518518518518517</v>
       </c>
     </row>
-    <row r="208" spans="1:33" ht="15">
+    <row r="208" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A208" s="37">
         <v>44480</v>
       </c>
@@ -32439,7 +32511,7 @@
         <v>-0.10967741935483867</v>
       </c>
     </row>
-    <row r="209" spans="1:33" ht="15">
+    <row r="209" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A209" s="37">
         <v>44481</v>
       </c>
@@ -32489,7 +32561,7 @@
         <v>-0.42622950819672129</v>
       </c>
     </row>
-    <row r="210" spans="1:33" ht="15">
+    <row r="210" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A210" s="37">
         <v>44482</v>
       </c>
@@ -32539,7 +32611,7 @@
         <v>0.17931034482758615</v>
       </c>
     </row>
-    <row r="211" spans="1:33" ht="15">
+    <row r="211" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A211" s="37">
         <v>44483</v>
       </c>
@@ -32589,7 +32661,7 @@
         <v>0.60869565217391308</v>
       </c>
     </row>
-    <row r="212" spans="1:33" ht="15">
+    <row r="212" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A212" s="37">
         <v>44484</v>
       </c>
@@ -32639,7 +32711,7 @@
         <v>-0.47590361445783136</v>
       </c>
     </row>
-    <row r="213" spans="1:33" ht="15">
+    <row r="213" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A213" s="37">
         <v>44487</v>
       </c>
@@ -32689,7 +32761,7 @@
         <v>0.40624999999999994</v>
       </c>
     </row>
-    <row r="214" spans="1:33">
+    <row r="214" spans="1:33" ht="15" x14ac:dyDescent="0.2">
       <c r="A214" s="37">
         <v>44488</v>
       </c>
@@ -32739,7 +32811,7 @@
         <v>0.11235955056179771</v>
       </c>
     </row>
-    <row r="215" spans="1:33">
+    <row r="215" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A215" s="37">
         <v>44489</v>
       </c>
@@ -32789,7 +32861,7 @@
         <v>-0.15294117647058819</v>
       </c>
     </row>
-    <row r="216" spans="1:33">
+    <row r="216" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A216" s="37">
         <v>44490</v>
       </c>
@@ -32839,7 +32911,7 @@
         <v>-0.36507936507936506</v>
       </c>
     </row>
-    <row r="217" spans="1:33">
+    <row r="217" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A217" s="37">
         <v>44491</v>
       </c>
@@ -32889,7 +32961,7 @@
         <v>-0.24025974025974028</v>
       </c>
     </row>
-    <row r="218" spans="1:33">
+    <row r="218" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A218" s="37">
         <v>44494</v>
       </c>
@@ -32939,7 +33011,7 @@
         <v>0.51181102362204711</v>
       </c>
     </row>
-    <row r="219" spans="1:33">
+    <row r="219" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A219" s="37">
         <v>44495</v>
       </c>
@@ -32989,7 +33061,7 @@
         <v>-0.34965034965034963</v>
       </c>
     </row>
-    <row r="220" spans="1:33">
+    <row r="220" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A220" s="37">
         <v>44496</v>
       </c>
@@ -33039,7 +33111,7 @@
         <v>-8.2089552238805916E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:33">
+    <row r="221" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A221" s="37">
         <v>44497</v>
       </c>
@@ -33089,7 +33161,7 @@
         <v>-0.13970588235294124</v>
       </c>
     </row>
-    <row r="222" spans="1:33">
+    <row r="222" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A222" s="37">
         <v>44498</v>
       </c>
@@ -33139,7 +33211,7 @@
         <v>0.83783783783783783</v>
       </c>
     </row>
-    <row r="223" spans="1:33">
+    <row r="223" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A223" s="37">
         <v>44501</v>
       </c>
@@ -33189,7 +33261,7 @@
         <v>0.84459459459459452</v>
       </c>
     </row>
-    <row r="224" spans="1:33">
+    <row r="224" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A224" s="37">
         <v>44502</v>
       </c>
@@ -33239,7 +33311,7 @@
         <v>-0.33333333333333331</v>
       </c>
     </row>
-    <row r="225" spans="1:33">
+    <row r="225" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A225" s="37">
         <v>44503</v>
       </c>
@@ -33289,7 +33361,7 @@
         <v>-0.30541871921182273</v>
       </c>
     </row>
-    <row r="226" spans="1:33">
+    <row r="226" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A226" s="37">
         <v>44504</v>
       </c>
@@ -33339,7 +33411,7 @@
         <v>0.59890109890109899</v>
       </c>
     </row>
-    <row r="227" spans="1:33">
+    <row r="227" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A227" s="37">
         <v>44505</v>
       </c>
@@ -33389,7 +33461,7 @@
         <v>-0.20212765957446804</v>
       </c>
     </row>
-    <row r="228" spans="1:33">
+    <row r="228" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A228" s="37">
         <v>44508</v>
       </c>
@@ -33439,7 +33511,7 @@
         <v>-0.1185567010309279</v>
       </c>
     </row>
-    <row r="229" spans="1:33">
+    <row r="229" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A229" s="37">
         <v>44509</v>
       </c>
@@ -33489,7 +33561,7 @@
         <v>-0.11764705882352941</v>
       </c>
     </row>
-    <row r="230" spans="1:33">
+    <row r="230" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A230" s="37">
         <v>44510</v>
       </c>
@@ -33539,7 +33611,7 @@
         <v>-0.15568862275449097</v>
       </c>
     </row>
-    <row r="231" spans="1:33">
+    <row r="231" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A231" s="37">
         <v>44511</v>
       </c>
@@ -33589,7 +33661,7 @@
         <v>0.29878048780487809</v>
       </c>
     </row>
-    <row r="232" spans="1:33">
+    <row r="232" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A232" s="37">
         <v>44512</v>
       </c>
@@ -33639,7 +33711,7 @@
         <v>0.41573033707865165</v>
       </c>
     </row>
-    <row r="233" spans="1:33">
+    <row r="233" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A233" s="37">
         <v>44515</v>
       </c>
@@ -33689,7 +33761,7 @@
         <v>0.14356435643564364</v>
       </c>
     </row>
-    <row r="234" spans="1:33">
+    <row r="234" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A234" s="37">
         <v>44516</v>
       </c>
@@ -33739,7 +33811,7 @@
         <v>-0.22413793103448271</v>
       </c>
     </row>
-    <row r="235" spans="1:33">
+    <row r="235" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A235" s="37">
         <v>44517</v>
       </c>
@@ -33789,7 +33861,7 @@
         <v>0.27601809954751122</v>
       </c>
     </row>
-    <row r="236" spans="1:33">
+    <row r="236" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A236" s="37">
         <v>44518</v>
       </c>
@@ -33839,7 +33911,7 @@
         <v>-0.33766233766233766</v>
       </c>
     </row>
-    <row r="237" spans="1:33">
+    <row r="237" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A237" s="37">
         <v>44519</v>
       </c>
@@ -33889,7 +33961,7 @@
         <v>9.7560975609756791E-3</v>
       </c>
     </row>
-    <row r="238" spans="1:33">
+    <row r="238" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A238" s="37">
         <v>44522</v>
       </c>
@@ -33939,7 +34011,7 @@
         <v>0.21962616822429915</v>
       </c>
     </row>
-    <row r="239" spans="1:33">
+    <row r="239" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A239" s="37">
         <v>44523</v>
       </c>
@@ -33989,7 +34061,7 @@
         <v>-0.14492753623188406</v>
       </c>
     </row>
-    <row r="240" spans="1:33">
+    <row r="240" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A240" s="37">
         <v>44524</v>
       </c>
@@ -34039,7 +34111,7 @@
         <v>8.8372093023255743E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:33">
+    <row r="241" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A241" s="37">
         <v>44525</v>
       </c>
@@ -34089,7 +34161,7 @@
         <v>-0.22321428571428575</v>
       </c>
     </row>
-    <row r="242" spans="1:33">
+    <row r="242" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A242" s="37">
         <v>44526</v>
       </c>
@@ -34139,7 +34211,7 @@
         <v>-0.2153846153846154</v>
       </c>
     </row>
-    <row r="243" spans="1:33">
+    <row r="243" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A243" s="37">
         <v>44529</v>
       </c>
@@ -34189,7 +34261,7 @@
         <v>0.12299465240641708</v>
       </c>
     </row>
-    <row r="244" spans="1:33">
+    <row r="244" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A244" s="37">
         <v>44530</v>
       </c>
@@ -34239,7 +34311,7 @@
         <v>0.17318435754189948</v>
       </c>
     </row>
-    <row r="245" spans="1:33">
+    <row r="245" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A245" s="37">
         <v>44531</v>
       </c>
@@ -34289,7 +34361,7 @@
         <v>0.33507853403141369</v>
       </c>
     </row>
-    <row r="246" spans="1:33">
+    <row r="246" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A246" s="37">
         <v>44532</v>
       </c>
@@ -34339,7 +34411,7 @@
         <v>-0.30666666666666664</v>
       </c>
     </row>
-    <row r="247" spans="1:33">
+    <row r="247" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A247" s="37">
         <v>44533</v>
       </c>
@@ -34389,7 +34461,7 @@
         <v>-0.20289855072463769</v>
       </c>
     </row>
-    <row r="248" spans="1:33">
+    <row r="248" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A248" s="37">
         <v>44536</v>
       </c>
@@ -34439,7 +34511,7 @@
         <v>-0.390625</v>
       </c>
     </row>
-    <row r="249" spans="1:33">
+    <row r="249" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A249" s="37">
         <v>44537</v>
       </c>
@@ -34489,7 +34561,7 @@
         <v>4.7945205479452108E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:33">
+    <row r="250" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A250" s="37">
         <v>44538</v>
       </c>
@@ -34539,7 +34611,7 @@
         <v>0.69655172413793098</v>
       </c>
     </row>
-    <row r="251" spans="1:33">
+    <row r="251" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A251" s="37">
         <v>44539</v>
       </c>
@@ -34589,7 +34661,7 @@
         <v>0.18604651162790692</v>
       </c>
     </row>
-    <row r="252" spans="1:33">
+    <row r="252" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A252" s="37">
         <v>44540</v>
       </c>
@@ -34639,7 +34711,7 @@
         <v>1.4925373134328358E-2</v>
       </c>
     </row>
-    <row r="253" spans="1:33">
+    <row r="253" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A253" s="37">
         <v>44543</v>
       </c>
@@ -34689,7 +34761,7 @@
         <v>8.7155963302752229E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:33">
+    <row r="254" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A254" s="37">
         <v>44544</v>
       </c>
@@ -34739,7 +34811,7 @@
         <v>0.2976744186046511</v>
       </c>
     </row>
-    <row r="255" spans="1:33">
+    <row r="255" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A255" s="37">
         <v>44545</v>
       </c>
@@ -34789,7 +34861,7 @@
         <v>-1.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="256" spans="1:33">
+    <row r="256" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A256" s="37">
         <v>44546</v>
       </c>
@@ -34839,7 +34911,7 @@
         <v>5.1792828685258904E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:33">
+    <row r="257" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A257" s="37">
         <v>44547</v>
       </c>
@@ -34889,7 +34961,7 @@
         <v>-1.9230769230769284E-2</v>
       </c>
     </row>
-    <row r="258" spans="1:33">
+    <row r="258" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A258" s="37">
         <v>44550</v>
       </c>
@@ -34939,7 +35011,7 @@
         <v>0.17857142857142858</v>
       </c>
     </row>
-    <row r="259" spans="1:33">
+    <row r="259" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A259" s="37">
         <v>44551</v>
       </c>
@@ -34989,7 +35061,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="260" spans="1:33">
+    <row r="260" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A260" s="37">
         <v>44552</v>
       </c>
@@ -35039,7 +35111,7 @@
         <v>-0.27812500000000001</v>
       </c>
     </row>
-    <row r="261" spans="1:33">
+    <row r="261" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A261" s="37">
         <v>44553</v>
       </c>
@@ -35089,7 +35161,7 @@
         <v>-0.32692307692307693</v>
       </c>
     </row>
-    <row r="262" spans="1:33">
+    <row r="262" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A262" s="37">
         <v>44554</v>
       </c>
@@ -35139,7 +35211,7 @@
         <v>-0.45936395759717313</v>
       </c>
     </row>
-    <row r="263" spans="1:33">
+    <row r="263" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A263" s="37">
         <v>44557</v>
       </c>
@@ -35189,7 +35261,7 @@
         <v>-6.0606060606060608E-2</v>
       </c>
     </row>
-    <row r="264" spans="1:33">
+    <row r="264" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A264" s="37">
         <v>44558</v>
       </c>
@@ -35239,7 +35311,7 @@
         <v>-3.2786885245901641E-2</v>
       </c>
     </row>
-    <row r="265" spans="1:33">
+    <row r="265" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A265" s="37">
         <v>44559</v>
       </c>
@@ -35289,7 +35361,7 @@
         <v>9.8837209302325535E-2</v>
       </c>
     </row>
-    <row r="266" spans="1:33">
+    <row r="266" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A266" s="37">
         <v>44560</v>
       </c>
@@ -35339,7 +35411,7 @@
         <v>0.40217391304347822</v>
       </c>
     </row>
-    <row r="267" spans="1:33">
+    <row r="267" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A267" s="37">
         <v>44561</v>
       </c>
@@ -35389,7 +35461,7 @@
         <v>-0.16346153846153841</v>
       </c>
     </row>
-    <row r="268" spans="1:33">
+    <row r="268" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A268" s="37">
         <v>44565</v>
       </c>
@@ -35439,7 +35511,7 @@
         <v>0.34782608695652173</v>
       </c>
     </row>
-    <row r="269" spans="1:33">
+    <row r="269" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A269" s="37">
         <v>44566</v>
       </c>
@@ -35489,7 +35561,7 @@
         <v>-0.39240506329113922</v>
       </c>
     </row>
-    <row r="270" spans="1:33">
+    <row r="270" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A270" s="37">
         <v>44567</v>
       </c>
@@ -35539,7 +35611,7 @@
         <v>0.25125628140703526</v>
       </c>
     </row>
-    <row r="271" spans="1:33">
+    <row r="271" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A271" s="37">
         <v>44568</v>
       </c>
@@ -35589,7 +35661,7 @@
         <v>-0.4241071428571429</v>
       </c>
     </row>
-    <row r="272" spans="1:33">
+    <row r="272" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A272" s="95">
         <v>44571</v>
       </c>
@@ -35657,7 +35729,7 @@
         <v>0.20689655172413793</v>
       </c>
     </row>
-    <row r="273" spans="1:33">
+    <row r="273" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A273" s="95">
         <v>44572</v>
       </c>
@@ -35725,7 +35797,7 @@
         <v>-0.14285714285714279</v>
       </c>
     </row>
-    <row r="274" spans="1:33">
+    <row r="274" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A274" s="95">
         <v>44573</v>
       </c>
@@ -35775,7 +35847,7 @@
         <v>0.63313609467455612</v>
       </c>
     </row>
-    <row r="275" spans="1:33">
+    <row r="275" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A275" s="95">
         <v>44574</v>
       </c>
@@ -35843,7 +35915,7 @@
         <v>-0.22935779816513766</v>
       </c>
     </row>
-    <row r="276" spans="1:33">
+    <row r="276" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A276" s="95">
         <v>44575</v>
       </c>
@@ -35911,7 +35983,7 @@
         <v>8.8235294117647065E-2</v>
       </c>
     </row>
-    <row r="277" spans="1:33">
+    <row r="277" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A277" s="95">
         <v>44578</v>
       </c>
@@ -35979,7 +36051,7 @@
         <v>0.47297297297297297</v>
       </c>
     </row>
-    <row r="278" spans="1:33">
+    <row r="278" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A278" s="37">
         <v>44579</v>
       </c>
@@ -36029,7 +36101,7 @@
         <v>-0.4853556485355649</v>
       </c>
     </row>
-    <row r="279" spans="1:33">
+    <row r="279" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A279" s="37">
         <v>44580</v>
       </c>
@@ -36079,7 +36151,7 @@
         <v>-0.25000000000000006</v>
       </c>
     </row>
-    <row r="280" spans="1:33">
+    <row r="280" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A280" s="37">
         <v>44581</v>
       </c>
@@ -36129,7 +36201,7 @@
         <v>-0.38834951456310685</v>
       </c>
     </row>
-    <row r="281" spans="1:33">
+    <row r="281" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A281" s="37">
         <v>44582</v>
       </c>
@@ -36179,7 +36251,7 @@
         <v>3.5971223021582684E-2</v>
       </c>
     </row>
-    <row r="282" spans="1:33">
+    <row r="282" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A282" s="37">
         <v>44585</v>
       </c>
@@ -36229,7 +36301,7 @@
         <v>0.10958904109589046</v>
       </c>
     </row>
-    <row r="283" spans="1:33">
+    <row r="283" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A283" s="37">
         <v>44586</v>
       </c>
@@ -36279,7 +36351,7 @@
         <v>-0.47916666666666669</v>
       </c>
     </row>
-    <row r="284" spans="1:33">
+    <row r="284" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A284" s="37">
         <v>44587</v>
       </c>
@@ -36329,7 +36401,7 @@
         <v>0.20472440944881884</v>
       </c>
     </row>
-    <row r="285" spans="1:33">
+    <row r="285" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A285" s="37">
         <v>44588</v>
       </c>
@@ -36379,7 +36451,7 @@
         <v>-0.70000000000000007</v>
       </c>
     </row>
-    <row r="286" spans="1:33">
+    <row r="286" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A286" s="37">
         <v>44589</v>
       </c>
@@ -36429,7 +36501,7 @@
         <v>0.88764044943820219</v>
       </c>
     </row>
-    <row r="287" spans="1:33">
+    <row r="287" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A287" s="37">
         <v>44599</v>
       </c>
@@ -36479,7 +36551,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="288" spans="1:33">
+    <row r="288" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A288" s="37">
         <v>44600</v>
       </c>
@@ -36529,7 +36601,7 @@
         <v>0.87741935483870981</v>
       </c>
     </row>
-    <row r="289" spans="1:33">
+    <row r="289" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A289" s="37">
         <v>44601</v>
       </c>
@@ -36579,7 +36651,7 @@
         <v>0.20502092050209197</v>
       </c>
     </row>
-    <row r="290" spans="1:33">
+    <row r="290" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A290" s="37">
         <v>44602</v>
       </c>
@@ -36629,7 +36701,7 @@
         <v>-0.39784946236559138</v>
       </c>
     </row>
-    <row r="291" spans="1:33">
+    <row r="291" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A291" s="37">
         <v>44603</v>
       </c>
@@ -36679,7 +36751,7 @@
         <v>-0.38554216867469882</v>
       </c>
     </row>
-    <row r="292" spans="1:33" ht="18">
+    <row r="292" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A292" s="37">
         <v>44606</v>
       </c>
@@ -36739,7 +36811,7 @@
         <v>0.24137931034482749</v>
       </c>
     </row>
-    <row r="293" spans="1:33" ht="18">
+    <row r="293" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A293" s="37">
         <v>44607</v>
       </c>
@@ -36799,7 +36871,7 @@
         <v>-0.12041884816753923</v>
       </c>
     </row>
-    <row r="294" spans="1:33" ht="18">
+    <row r="294" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A294" s="37">
         <v>44608</v>
       </c>
@@ -36859,7 +36931,7 @@
         <v>0.130890052356021</v>
       </c>
     </row>
-    <row r="295" spans="1:33" ht="18">
+    <row r="295" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A295" s="37">
         <v>44609</v>
       </c>
@@ -36919,7 +36991,7 @@
         <v>-0.36320754716981135</v>
       </c>
     </row>
-    <row r="296" spans="1:33" ht="18">
+    <row r="296" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A296" s="37">
         <v>44610</v>
       </c>
@@ -36979,7 +37051,7 @@
         <v>-9.826589595375719E-2</v>
       </c>
     </row>
-    <row r="297" spans="1:33" ht="18">
+    <row r="297" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A297" s="37">
         <v>44613</v>
       </c>
@@ -37039,7 +37111,7 @@
         <v>0.7751479289940828</v>
       </c>
     </row>
-    <row r="298" spans="1:33" ht="18">
+    <row r="298" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A298" s="37">
         <v>44614</v>
       </c>
@@ -37099,7 +37171,7 @@
         <v>-0.22335025380710666</v>
       </c>
     </row>
-    <row r="299" spans="1:33" ht="18">
+    <row r="299" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A299" s="37">
         <v>44615</v>
       </c>
@@ -37159,7 +37231,7 @@
         <v>0.31527093596059103</v>
       </c>
     </row>
-    <row r="300" spans="1:33" ht="18">
+    <row r="300" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A300" s="37">
         <v>44616</v>
       </c>
@@ -37219,7 +37291,7 @@
         <v>-0.52500000000000002</v>
       </c>
     </row>
-    <row r="301" spans="1:33" ht="18">
+    <row r="301" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A301" s="37">
         <v>44617</v>
       </c>
@@ -37279,7 +37351,7 @@
         <v>1.1235955056179735E-2</v>
       </c>
     </row>
-    <row r="302" spans="1:33" ht="18">
+    <row r="302" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A302" s="37">
         <v>44620</v>
       </c>
@@ -37339,7 +37411,7 @@
         <v>-0.27807486631016043</v>
       </c>
     </row>
-    <row r="303" spans="1:33" ht="18">
+    <row r="303" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A303" s="37">
         <v>44621</v>
       </c>
@@ -37399,7 +37471,7 @@
         <v>0.11188811188811194</v>
       </c>
     </row>
-    <row r="304" spans="1:33" ht="18">
+    <row r="304" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A304" s="37">
         <v>44622</v>
       </c>
@@ -37459,7 +37531,7 @@
         <v>0.21518987341772158</v>
       </c>
     </row>
-    <row r="305" spans="1:33" ht="18">
+    <row r="305" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A305" s="37">
         <v>44623</v>
       </c>
@@ -37519,7 +37591,7 @@
         <v>0.40740740740740738</v>
       </c>
     </row>
-    <row r="306" spans="1:33" ht="18">
+    <row r="306" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A306" s="37">
         <v>44624</v>
       </c>
@@ -37579,7 +37651,7 @@
         <v>-0.30051813471502586</v>
       </c>
     </row>
-    <row r="307" spans="1:33" ht="18">
+    <row r="307" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A307" s="37">
         <v>44627</v>
       </c>
@@ -37639,7 +37711,7 @@
         <v>-0.15675675675675674</v>
       </c>
     </row>
-    <row r="308" spans="1:33" ht="18">
+    <row r="308" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A308" s="37">
         <v>44628</v>
       </c>
@@ -37699,7 +37771,7 @@
         <v>-0.63583815028901736</v>
       </c>
     </row>
-    <row r="309" spans="1:33" s="23" customFormat="1" ht="18">
+    <row r="309" spans="1:33" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A309" s="22">
         <v>44629</v>
       </c>
@@ -37767,7 +37839,7 @@
         <v>0.16949152542372875</v>
       </c>
     </row>
-    <row r="310" spans="1:33" ht="18">
+    <row r="310" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A310" s="37">
         <v>44630</v>
       </c>
@@ -37827,7 +37899,7 @@
         <v>1.1176470588235294</v>
       </c>
     </row>
-    <row r="311" spans="1:33" ht="18">
+    <row r="311" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A311" s="37">
         <v>44631</v>
       </c>
@@ -37887,7 +37959,7 @@
         <v>0.37086092715231783</v>
       </c>
     </row>
-    <row r="312" spans="1:33" ht="18">
+    <row r="312" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A312" s="37">
         <v>44634</v>
       </c>
@@ -37947,7 +38019,7 @@
         <v>-0.35175879396984921</v>
       </c>
     </row>
-    <row r="313" spans="1:33" s="23" customFormat="1" ht="18">
+    <row r="313" spans="1:33" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A313" s="22">
         <v>44635</v>
       </c>
@@ -38015,7 +38087,7 @@
         <v>-0.54081632653061218</v>
       </c>
     </row>
-    <row r="314" spans="1:33" ht="18">
+    <row r="314" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A314" s="37">
         <v>44636</v>
       </c>
@@ -38075,7 +38147,7 @@
         <v>1.7464788732394363</v>
       </c>
     </row>
-    <row r="315" spans="1:33" ht="18">
+    <row r="315" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A315" s="37">
         <v>44637</v>
       </c>
@@ -38135,7 +38207,7 @@
         <v>0.46305418719211811</v>
       </c>
     </row>
-    <row r="316" spans="1:33" ht="18">
+    <row r="316" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A316" s="37">
         <v>44638</v>
       </c>
@@ -38195,7 +38267,7 @@
         <v>0.22779922779922787</v>
       </c>
     </row>
-    <row r="317" spans="1:33" ht="18">
+    <row r="317" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A317" s="37">
         <v>44641</v>
       </c>
@@ -38255,7 +38327,7 @@
         <v>3.8805970149253688E-2</v>
       </c>
     </row>
-    <row r="318" spans="1:33" ht="18">
+    <row r="318" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A318" s="37">
         <v>44642</v>
       </c>
@@ -38315,7 +38387,7 @@
         <v>-0.26168224299065418</v>
       </c>
     </row>
-    <row r="319" spans="1:33" ht="18">
+    <row r="319" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A319" s="37">
         <v>44643</v>
       </c>
@@ -38375,7 +38447,7 @@
         <v>-0.3122923588039867</v>
       </c>
     </row>
-    <row r="320" spans="1:33" ht="18">
+    <row r="320" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A320" s="37">
         <v>44644</v>
       </c>
@@ -38435,7 +38507,7 @@
         <v>-0.28409090909090912</v>
       </c>
     </row>
-    <row r="321" spans="1:33" ht="18">
+    <row r="321" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A321" s="37">
         <v>44645</v>
       </c>
@@ -38495,7 +38567,7 @@
         <v>6.6350710900474008E-2</v>
       </c>
     </row>
-    <row r="322" spans="1:33" ht="18">
+    <row r="322" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A322" s="37">
         <v>44648</v>
       </c>
@@ -38555,7 +38627,7 @@
         <v>-0.10144927536231885</v>
       </c>
     </row>
-    <row r="323" spans="1:33" ht="18">
+    <row r="323" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A323" s="37">
         <v>44649</v>
       </c>
@@ -38615,7 +38687,7 @@
         <v>-0.16000000000000006</v>
       </c>
     </row>
-    <row r="324" spans="1:33" ht="18">
+    <row r="324" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A324" s="37">
         <v>44650</v>
       </c>
@@ -38675,7 +38747,7 @@
         <v>0.24352331606217625</v>
       </c>
     </row>
-    <row r="325" spans="1:33" ht="18">
+    <row r="325" spans="1:33" ht="19" x14ac:dyDescent="0.2">
       <c r="A325" s="37">
         <v>44651</v>
       </c>
@@ -38735,7 +38807,7 @@
         <v>-0.16666666666666666</v>
       </c>
     </row>
-    <row r="326" spans="1:33">
+    <row r="326" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A326" s="37">
         <v>44652</v>
       </c>
@@ -38787,7 +38859,7 @@
         <v>0.130890052356021</v>
       </c>
     </row>
-    <row r="327" spans="1:33">
+    <row r="327" spans="1:33" ht="15" x14ac:dyDescent="0.2">
       <c r="A327" s="37">
         <v>44657</v>
       </c>
@@ -38837,7 +38909,7 @@
         <v>0.18840579710144928</v>
       </c>
     </row>
-    <row r="328" spans="1:33">
+    <row r="328" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A328" s="37">
         <v>44658</v>
       </c>
@@ -38887,7 +38959,7 @@
         <v>-0.54066985645933019</v>
       </c>
     </row>
-    <row r="329" spans="1:33">
+    <row r="329" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A329" s="37">
         <v>44659</v>
       </c>
@@ -38937,7 +39009,7 @@
         <v>3.2258064516129031E-2</v>
       </c>
     </row>
-    <row r="330" spans="1:33">
+    <row r="330" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A330" s="37">
         <v>44662</v>
       </c>
@@ -38987,7 +39059,7 @@
         <v>-0.1067415730337079</v>
       </c>
     </row>
-    <row r="331" spans="1:33">
+    <row r="331" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A331" s="37">
         <v>44663</v>
       </c>
@@ -39037,7 +39109,7 @@
         <v>0.93288590604026855</v>
       </c>
     </row>
-    <row r="332" spans="1:33">
+    <row r="332" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A332" s="37">
         <v>44664</v>
       </c>
@@ -39087,7 +39159,7 @@
         <v>-0.25352112676056338</v>
       </c>
     </row>
-    <row r="333" spans="1:33">
+    <row r="333" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A333" s="37">
         <v>44665</v>
       </c>
@@ -39137,7 +39209,7 @@
         <v>0.14356435643564364</v>
       </c>
     </row>
-    <row r="334" spans="1:33">
+    <row r="334" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A334" s="37">
         <v>44666</v>
       </c>
@@ -39187,7 +39259,7 @@
         <v>-0.49557522123893805</v>
       </c>
     </row>
-    <row r="335" spans="1:33">
+    <row r="335" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A335" s="37">
         <v>44669</v>
       </c>
@@ -39237,7 +39309,7 @@
         <v>0.35714285714285715</v>
       </c>
     </row>
-    <row r="336" spans="1:33">
+    <row r="336" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A336" s="37">
         <v>44670</v>
       </c>
@@ -39287,7 +39359,7 @@
         <v>-0.12041884816753923</v>
       </c>
     </row>
-    <row r="337" spans="1:33">
+    <row r="337" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A337" s="37">
         <v>44671</v>
       </c>
@@ -39335,6 +39407,106 @@
       <c r="AG337" s="110">
         <f t="shared" ref="AG337" si="50">(B337-AF337)/AF337</f>
         <v>-8.2352941176470545E-2</v>
+      </c>
+    </row>
+    <row r="338" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A338" s="37">
+        <v>44672</v>
+      </c>
+      <c r="B338" s="38">
+        <v>32</v>
+      </c>
+      <c r="C338" s="38">
+        <v>15</v>
+      </c>
+      <c r="D338" s="38">
+        <v>-90</v>
+      </c>
+      <c r="E338" s="38">
+        <v>-66</v>
+      </c>
+      <c r="F338" s="38">
+        <v>-1963</v>
+      </c>
+      <c r="G338" s="38">
+        <v>-1344</v>
+      </c>
+      <c r="H338" s="38">
+        <v>-250</v>
+      </c>
+      <c r="I338" s="39">
+        <f t="shared" ref="I338" si="51">B338/(B338+C338)*100</f>
+        <v>68.085106382978722</v>
+      </c>
+      <c r="J338" s="39">
+        <v>-0.86</v>
+      </c>
+      <c r="K338" s="39">
+        <v>-1.85</v>
+      </c>
+      <c r="T338" s="94">
+        <v>5</v>
+      </c>
+      <c r="U338" s="43">
+        <v>4</v>
+      </c>
+      <c r="AF338" s="109">
+        <f t="shared" ref="AF338" si="52">(B335+B336+B337)/3</f>
+        <v>61.333333333333336</v>
+      </c>
+      <c r="AG338" s="110">
+        <f t="shared" ref="AG338" si="53">(B338-AF338)/AF338</f>
+        <v>-0.47826086956521741</v>
+      </c>
+    </row>
+    <row r="339" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A339" s="37">
+        <v>44673</v>
+      </c>
+      <c r="B339" s="38">
+        <v>75</v>
+      </c>
+      <c r="C339" s="38">
+        <v>10</v>
+      </c>
+      <c r="D339" s="38">
+        <v>-85</v>
+      </c>
+      <c r="E339" s="38">
+        <v>-65</v>
+      </c>
+      <c r="F339" s="38">
+        <v>-665</v>
+      </c>
+      <c r="G339" s="38">
+        <v>-383</v>
+      </c>
+      <c r="H339" s="38">
+        <v>-250</v>
+      </c>
+      <c r="I339" s="39">
+        <f t="shared" ref="I339" si="54">B339/(B339+C339)*100</f>
+        <v>88.235294117647058</v>
+      </c>
+      <c r="J339" s="39">
+        <v>2.63</v>
+      </c>
+      <c r="K339" s="39">
+        <v>0.19</v>
+      </c>
+      <c r="T339" s="94">
+        <v>5</v>
+      </c>
+      <c r="U339" s="43">
+        <v>3</v>
+      </c>
+      <c r="AF339" s="109">
+        <f t="shared" ref="AF339" si="55">(B336+B337+B338)/3</f>
+        <v>46.666666666666664</v>
+      </c>
+      <c r="AG339" s="110">
+        <f t="shared" ref="AG339" si="56">(B339-AF339)/AF339</f>
+        <v>0.60714285714285721</v>
       </c>
     </row>
   </sheetData>
@@ -39345,7 +39517,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="8" id="{AA3D4853-DFC7-A44C-AAF4-ED502B2966F5}">
+          <x14:cfRule type="iconSet" priority="20" id="{AA3D4853-DFC7-A44C-AAF4-ED502B2966F5}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -39361,10 +39533,10 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>I1:I1048576</xm:sqref>
+          <xm:sqref>I1:I337 I340:I1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="7" id="{5668E6E0-C4AC-C442-9BCB-A9B3CB042970}">
+          <x14:cfRule type="iconSet" priority="19" id="{5668E6E0-C4AC-C442-9BCB-A9B3CB042970}">
             <x14:iconSet iconSet="3Arrows" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -39380,10 +39552,10 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>B1:B327 B330:B1048576 C328</xm:sqref>
+          <xm:sqref>B1:B327 B330:B337 C328 B340:B1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="5" id="{CC481063-6BD0-3947-B031-AA136F500496}">
+          <x14:cfRule type="iconSet" priority="17" id="{CC481063-6BD0-3947-B031-AA136F500496}">
             <x14:iconSet iconSet="3Arrows" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -39399,10 +39571,10 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>D1:D327 D330:D333 D335:D1048576 E334 E328</xm:sqref>
+          <xm:sqref>D1:D327 D330:D333 D335:D337 E334 E328 D340:D1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="4" id="{DF774614-C12F-4C4F-9792-6234D19AF46D}">
+          <x14:cfRule type="iconSet" priority="16" id="{DF774614-C12F-4C4F-9792-6234D19AF46D}">
             <x14:iconSet iconSet="3Arrows" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -39418,10 +39590,10 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>E1:E327 E330:E333 E335:E1048576 F334 F328</xm:sqref>
+          <xm:sqref>E1:E327 E330:E333 E335:E337 F334 F328 E340:E1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="3" id="{8CB41595-F9EE-3547-A26F-50C5E7A82163}">
+          <x14:cfRule type="iconSet" priority="15" id="{8CB41595-F9EE-3547-A26F-50C5E7A82163}">
             <x14:iconSet iconSet="3Arrows" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -39437,10 +39609,10 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>F1:F327 F330:F333 F335:F1048576</xm:sqref>
+          <xm:sqref>F1:F327 F330:F333 F335:F337 F340:F1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="2" id="{FF4E5384-FA77-554B-A82C-5F6FE16203A1}">
+          <x14:cfRule type="iconSet" priority="14" id="{FF4E5384-FA77-554B-A82C-5F6FE16203A1}">
             <x14:iconSet iconSet="3Arrows" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -39456,10 +39628,10 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>G1:G328 G330:G1048576</xm:sqref>
+          <xm:sqref>G1:G328 G330:G337 G340:G1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{39F9903C-C6F9-E74E-A92D-D03599FF392A}">
+          <x14:cfRule type="iconSet" priority="13" id="{39F9903C-C6F9-E74E-A92D-D03599FF392A}">
             <x14:iconSet iconSet="3Arrows" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -39477,10 +39649,235 @@
           </x14:cfRule>
           <xm:sqref>D329:H329</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="12" id="{32167799-798C-B84B-BD3E-21CC5214DCAE}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>60</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>80</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>I338</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="11" id="{784BE4FB-D14A-F644-8D12-23AB6ACB7C21}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>40</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>80</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B338</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="10" id="{5A51FD30-DEBA-D241-B767-3907EA3D3E90}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-38</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-10</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>D338</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="9" id="{9AB3A5A1-EF05-DF4A-B5EB-7C588B26A041}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-20</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-4</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>E338</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="8" id="{96DC5578-8FF9-8846-B7AF-6E3AC92E9EC0}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-470</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-200</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>F338</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="7" id="{7BF40097-502A-244B-9B20-FE1D1D77B24F}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-450</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-50</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>G338</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="6" id="{DE518C7D-DEBF-0B44-B3F9-736BC3550BDA}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>60</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>80</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>I339</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="5" id="{CDBF4A67-DC6D-F54F-AA87-E2FC07B641BE}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>40</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>80</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B339</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="4" id="{79D62743-7ECE-4C45-BAFA-B79DB5E11C97}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-38</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-10</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>D339</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="3" id="{4D119ABD-7F94-4F4A-9B70-A83FD73BD20C}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-20</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-4</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>E339</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="2" id="{FAFF466E-2732-4944-9199-4029121A66B4}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-470</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-200</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>F339</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{B83AEE10-19BA-8C40-AAA1-BDC41326DFCE}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-450</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-50</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>G339</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
@@ -39494,35 +39891,35 @@
       <selection activeCell="ZA6150" sqref="ZA6150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" customWidth="1"/>
-    <col min="6" max="7" width="24.85546875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" customWidth="1"/>
-    <col min="9" max="9" width="24.85546875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="32.140625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="31.140625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" hidden="1" customWidth="1"/>
-    <col min="13" max="15" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.1640625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
+    <col min="6" max="7" width="24.83203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="26.1640625" customWidth="1"/>
+    <col min="9" max="9" width="24.83203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="32.1640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="31.1640625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" hidden="1" customWidth="1"/>
+    <col min="13" max="15" width="24.83203125" customWidth="1"/>
     <col min="16" max="16" width="24" customWidth="1"/>
     <col min="17" max="17" width="25" customWidth="1"/>
-    <col min="18" max="18" width="20.140625" customWidth="1"/>
-    <col min="19" max="19" width="23.85546875" customWidth="1"/>
+    <col min="18" max="18" width="20.1640625" customWidth="1"/>
+    <col min="19" max="19" width="23.83203125" customWidth="1"/>
     <col min="20" max="20" width="26" customWidth="1"/>
-    <col min="21" max="21" width="24.85546875" customWidth="1"/>
-    <col min="22" max="22" width="22.140625" customWidth="1"/>
-    <col min="23" max="23" width="20.140625" customWidth="1"/>
-    <col min="24" max="24" width="32.140625" customWidth="1"/>
-    <col min="25" max="25" width="19.140625" customWidth="1"/>
-    <col min="26" max="26" width="29.42578125" customWidth="1"/>
-    <col min="27" max="27" width="23.85546875" customWidth="1"/>
+    <col min="21" max="21" width="24.83203125" customWidth="1"/>
+    <col min="22" max="22" width="22.1640625" customWidth="1"/>
+    <col min="23" max="23" width="20.1640625" customWidth="1"/>
+    <col min="24" max="24" width="32.1640625" customWidth="1"/>
+    <col min="25" max="25" width="19.1640625" customWidth="1"/>
+    <col min="26" max="26" width="29.5" customWidth="1"/>
+    <col min="27" max="27" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:27" ht="22">
+    <row r="2" spans="1:27" ht="23" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44305</v>
       </c>
@@ -39605,7 +40002,7 @@
         <v>44344</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="27">
+    <row r="3" spans="1:27" ht="28" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -39688,7 +40085,7 @@
         <v>1.34E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="27">
+    <row r="4" spans="1:27" ht="28" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="7" t="s">
         <v>37</v>
@@ -39769,7 +40166,7 @@
         <v>-7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="27">
+    <row r="5" spans="1:27" ht="28" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="6" t="s">
@@ -39848,7 +40245,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="27">
+    <row r="6" spans="1:27" ht="28" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -39925,7 +40322,7 @@
         <v>-2.52E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="27">
+    <row r="7" spans="1:27" ht="28" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -39996,7 +40393,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="27">
+    <row r="8" spans="1:27" ht="28" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -40067,7 +40464,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="22">
+    <row r="9" spans="1:27" ht="23" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -40112,7 +40509,7 @@
       <c r="Z9" s="6"/>
       <c r="AA9" s="6"/>
     </row>
-    <row r="10" spans="1:27" ht="22">
+    <row r="10" spans="1:27" ht="23" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -40159,7 +40556,7 @@
       <c r="Z10" s="6"/>
       <c r="AA10" s="6"/>
     </row>
-    <row r="11" spans="1:27" ht="22">
+    <row r="11" spans="1:27" ht="23" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -40206,7 +40603,7 @@
       <c r="Z11" s="6"/>
       <c r="AA11" s="6"/>
     </row>
-    <row r="12" spans="1:27" ht="27">
+    <row r="12" spans="1:27" ht="28" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -40259,7 +40656,7 @@
         <v>-3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="22">
+    <row r="13" spans="1:27" ht="23" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -40310,7 +40707,7 @@
       </c>
       <c r="AA13" s="6"/>
     </row>
-    <row r="14" spans="1:27" ht="22">
+    <row r="14" spans="1:27" ht="23" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -40359,7 +40756,7 @@
         <v>-5.7200000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="22">
+    <row r="15" spans="1:27" ht="23" x14ac:dyDescent="0.2">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -40406,7 +40803,7 @@
         <v>-1.1299999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="22">
+    <row r="16" spans="1:27" ht="23" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -40445,7 +40842,7 @@
         <v>-2.1700000000000001E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="22">
+    <row r="17" spans="1:27" ht="23" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -40484,7 +40881,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="22">
+    <row r="18" spans="1:27" ht="23" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -40524,10 +40921,5 @@
   </sheetData>
   <phoneticPr fontId="26" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: magic & date - 20220501
</commit_message>
<xml_diff>
--- a/magic_excel.xlsx
+++ b/magic_excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11200" yWindow="0" windowWidth="22320" windowHeight="19400"/>
+    <workbookView xWindow="15840" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="图" sheetId="3" r:id="rId1"/>
@@ -806,7 +806,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -832,6 +832,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1054,19 +1072,25 @@
     <xf numFmtId="179" fontId="18" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="2" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="19">
     <cellStyle name="百分比" xfId="1" builtinId="5"/>
     <cellStyle name="超链接" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="逗号" xfId="8" builtinId="3"/>
     <cellStyle name="访问过的超链接" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1205,10 +1229,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>情绪数据!$A$2:$A$2000</c:f>
+              <c:f>情绪数据!$A$2:$A$1998</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="1999"/>
+                <c:ptCount val="1997"/>
                 <c:pt idx="0">
                   <c:v>44165.0</c:v>
                 </c:pt>
@@ -2219,16 +2243,34 @@
                 </c:pt>
                 <c:pt idx="336">
                   <c:v>44672.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>44673.0</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>44676.0</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>44677.0</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>44678.0</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>44679.0</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>44680.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$T$2:$T$338</c:f>
+              <c:f>情绪数据!$T$2:$T$344</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="337"/>
+                <c:ptCount val="343"/>
                 <c:pt idx="0">
                   <c:v>4.0</c:v>
                 </c:pt>
@@ -3239,6 +3281,24 @@
                 </c:pt>
                 <c:pt idx="336">
                   <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>6.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3253,8 +3313,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2131811416"/>
-        <c:axId val="-2132100104"/>
+        <c:axId val="2086132344"/>
+        <c:axId val="2086006184"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4331,10 +4391,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$U$2:$U$338</c:f>
+              <c:f>情绪数据!$U$2:$U$344</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="337"/>
+                <c:ptCount val="343"/>
                 <c:pt idx="0">
                   <c:v>3.0</c:v>
                 </c:pt>
@@ -5344,6 +5404,24 @@
                   <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="336">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="342">
                   <c:v>4.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -5361,8 +5439,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2131811416"/>
-        <c:axId val="-2132100104"/>
+        <c:axId val="2086132344"/>
+        <c:axId val="2086006184"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6397,10 +6475,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$J$2:$J$338</c:f>
+              <c:f>情绪数据!$J$2:$J$344</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="337"/>
+                <c:ptCount val="343"/>
                 <c:pt idx="0">
                   <c:v>1.8</c:v>
                 </c:pt>
@@ -7411,6 +7489,24 @@
                 </c:pt>
                 <c:pt idx="336">
                   <c:v>-0.86</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>-6.38</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>-2.72</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>3.67</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>5.59</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8461,10 +8557,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$K$2:$K$338</c:f>
+              <c:f>情绪数据!$K$2:$K$344</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ ;[Red]\-0.00\ </c:formatCode>
-                <c:ptCount val="337"/>
+                <c:ptCount val="343"/>
                 <c:pt idx="0">
                   <c:v>-0.54</c:v>
                 </c:pt>
@@ -9475,6 +9571,24 @@
                 </c:pt>
                 <c:pt idx="336">
                   <c:v>-1.85</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>-6.12</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>-4.02</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>-0.25</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>2.05</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>4.61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9491,11 +9605,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2132096376"/>
-        <c:axId val="-2132093432"/>
+        <c:axId val="2086029496"/>
+        <c:axId val="2086184664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2131811416"/>
+        <c:axId val="2086132344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9563,7 +9677,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132100104"/>
+        <c:crossAx val="2086006184"/>
         <c:crossesAt val="0.0"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -9571,7 +9685,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2132100104"/>
+        <c:axId val="2086006184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9622,13 +9736,13 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2131811416"/>
+        <c:crossAx val="2086132344"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1.0"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-2132096376"/>
+        <c:axId val="2086029496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9638,7 +9752,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132093432"/>
+        <c:crossAx val="2086184664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -9646,7 +9760,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2132093432"/>
+        <c:axId val="2086184664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9683,7 +9797,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2132096376"/>
+        <c:crossAx val="2086029496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9787,10 +9901,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>情绪数据!$A$2:$A$2000</c:f>
+              <c:f>情绪数据!$A$2:$A$1998</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="1999"/>
+                <c:ptCount val="1997"/>
                 <c:pt idx="0">
                   <c:v>44165.0</c:v>
                 </c:pt>
@@ -10801,16 +10915,34 @@
                 </c:pt>
                 <c:pt idx="336">
                   <c:v>44672.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>44673.0</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>44676.0</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>44677.0</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>44678.0</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>44679.0</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>44680.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$B$2:$B$338</c:f>
+              <c:f>情绪数据!$B$2:$B$344</c:f>
               <c:numCache>
                 <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
-                <c:ptCount val="337"/>
+                <c:ptCount val="343"/>
                 <c:pt idx="0">
                   <c:v>26.0</c:v>
                 </c:pt>
@@ -11821,6 +11953,24 @@
                 </c:pt>
                 <c:pt idx="336">
                   <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>75.0</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>137.0</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>214.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11854,10 +12004,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>情绪数据!$A$2:$A$2000</c:f>
+              <c:f>情绪数据!$A$2:$A$1998</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="1999"/>
+                <c:ptCount val="1997"/>
                 <c:pt idx="0">
                   <c:v>44165.0</c:v>
                 </c:pt>
@@ -12868,16 +13018,34 @@
                 </c:pt>
                 <c:pt idx="336">
                   <c:v>44672.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>44673.0</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>44676.0</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>44677.0</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>44678.0</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>44679.0</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>44680.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$C$2:$C$338</c:f>
+              <c:f>情绪数据!$C$2:$C$344</c:f>
               <c:numCache>
                 <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
-                <c:ptCount val="337"/>
+                <c:ptCount val="343"/>
                 <c:pt idx="0">
                   <c:v>30.0</c:v>
                 </c:pt>
@@ -13888,6 +14056,24 @@
                 </c:pt>
                 <c:pt idx="336">
                   <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>31.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13901,8 +14087,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2134481848"/>
-        <c:axId val="-2134477992"/>
+        <c:axId val="2083331976"/>
+        <c:axId val="2083335896"/>
       </c:areaChart>
       <c:areaChart>
         <c:grouping val="stacked"/>
@@ -13934,10 +14120,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>情绪数据!$A$2:$A$327</c:f>
+              <c:f>情绪数据!$A$2:$A$344</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="326"/>
+                <c:ptCount val="343"/>
                 <c:pt idx="0">
                   <c:v>44165.0</c:v>
                 </c:pt>
@@ -14915,16 +15101,67 @@
                 </c:pt>
                 <c:pt idx="325">
                   <c:v>44657.0</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>44658.0</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>44659.0</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>44662.0</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>44663.0</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>44664.0</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>44665.0</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>44666.0</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>44669.0</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>44670.0</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>44671.0</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>44672.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>44673.0</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>44676.0</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>44677.0</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>44678.0</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>44679.0</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>44680.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$D$2:$D$338</c:f>
+              <c:f>情绪数据!$D$2:$D$344</c:f>
               <c:numCache>
                 <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
-                <c:ptCount val="337"/>
+                <c:ptCount val="343"/>
                 <c:pt idx="0">
                   <c:v>-17.0</c:v>
                 </c:pt>
@@ -15935,6 +16172,24 @@
                 </c:pt>
                 <c:pt idx="336">
                   <c:v>-90.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>-88.0</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>-677.0</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>-272.0</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>-148.0</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>-73.0</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>-18.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15968,10 +16223,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>情绪数据!$A$2:$A$327</c:f>
+              <c:f>情绪数据!$A$2:$A$344</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="326"/>
+                <c:ptCount val="343"/>
                 <c:pt idx="0">
                   <c:v>44165.0</c:v>
                 </c:pt>
@@ -16949,16 +17204,67 @@
                 </c:pt>
                 <c:pt idx="325">
                   <c:v>44657.0</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>44658.0</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>44659.0</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>44662.0</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>44663.0</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>44664.0</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>44665.0</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>44666.0</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>44669.0</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>44670.0</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>44671.0</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>44672.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>44673.0</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>44676.0</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>44677.0</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>44678.0</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>44679.0</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>44680.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$F$2:$F$338</c:f>
+              <c:f>情绪数据!$F$2:$F$344</c:f>
               <c:numCache>
                 <c:formatCode>0_ ;[Red]\-0\ </c:formatCode>
-                <c:ptCount val="337"/>
+                <c:ptCount val="343"/>
                 <c:pt idx="0">
                   <c:v>-158.0</c:v>
                 </c:pt>
@@ -17969,6 +18275,24 @@
                 </c:pt>
                 <c:pt idx="336">
                   <c:v>-1963.0</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>-665.0</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>-3993.0</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>-2044.0</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>-1271.0</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>-1334.0</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>-185.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17982,8 +18306,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2134474264"/>
-        <c:axId val="-2134471288"/>
+        <c:axId val="2083340216"/>
+        <c:axId val="2083343224"/>
       </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -19003,10 +19327,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>情绪数据!$AF$2:$AF$338</c:f>
+              <c:f>情绪数据!$AF$2:$AF$344</c:f>
               <c:numCache>
                 <c:formatCode>0.00_ </c:formatCode>
-                <c:ptCount val="337"/>
+                <c:ptCount val="343"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -20017,6 +20341,24 @@
                 </c:pt>
                 <c:pt idx="336">
                   <c:v>61.33333333333334</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>46.66666666666666</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>47.33333333333334</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>82.33333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20033,11 +20375,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2134481848"/>
-        <c:axId val="-2134477992"/>
+        <c:axId val="2083331976"/>
+        <c:axId val="2083335896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2134481848"/>
+        <c:axId val="2083331976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20091,7 +20433,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2134477992"/>
+        <c:crossAx val="2083335896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -20099,7 +20441,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2134477992"/>
+        <c:axId val="2083335896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="350.0"/>
@@ -20148,12 +20490,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2134481848"/>
+        <c:crossAx val="2083331976"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-2134474264"/>
+        <c:axId val="2083340216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20163,7 +20505,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2134471288"/>
+        <c:crossAx val="2083343224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -20171,7 +20513,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2134471288"/>
+        <c:axId val="2083343224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.0"/>
@@ -20207,7 +20549,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2134474264"/>
+        <c:crossAx val="2083340216"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -21684,8 +22026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="T33:CZ70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BL2" zoomScale="90" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="BZ16" sqref="BZ16"/>
+    <sheetView topLeftCell="BQ1" zoomScale="90" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="BZ24" sqref="BZ24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -21728,11 +22070,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG338"/>
+  <dimension ref="A1:AG344"/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K340" sqref="K340"/>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A323" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F340" sqref="F340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -35651,7 +35993,7 @@
         <v>-250</v>
       </c>
       <c r="I272" s="97">
-        <f t="shared" ref="I272:I338" si="26">B272/(B272+C272)*100</f>
+        <f t="shared" ref="I272:I340" si="26">B272/(B272+C272)*100</f>
         <v>81.395348837209298</v>
       </c>
       <c r="J272" s="97">
@@ -39421,6 +39763,306 @@
       <c r="AG338" s="110">
         <f t="shared" ref="AG338" si="52">(B338-AF338)/AF338</f>
         <v>-0.47826086956521741</v>
+      </c>
+    </row>
+    <row r="339" spans="1:33" ht="16" customHeight="1">
+      <c r="A339" s="37">
+        <v>44673</v>
+      </c>
+      <c r="B339" s="38">
+        <v>75</v>
+      </c>
+      <c r="C339" s="38">
+        <v>10</v>
+      </c>
+      <c r="D339" s="38">
+        <v>-88</v>
+      </c>
+      <c r="E339" s="38">
+        <v>-65</v>
+      </c>
+      <c r="F339" s="38">
+        <v>-665</v>
+      </c>
+      <c r="G339" s="38">
+        <v>-383</v>
+      </c>
+      <c r="H339" s="38">
+        <v>-250</v>
+      </c>
+      <c r="I339" s="39">
+        <f t="shared" si="26"/>
+        <v>88.235294117647058</v>
+      </c>
+      <c r="J339" s="39">
+        <v>-6.38</v>
+      </c>
+      <c r="K339" s="39">
+        <v>-6.12</v>
+      </c>
+      <c r="T339" s="94">
+        <v>5</v>
+      </c>
+      <c r="U339" s="43">
+        <v>3</v>
+      </c>
+      <c r="AF339" s="109">
+        <f t="shared" ref="AF339:AF341" si="53">(B336+B337+B338)/3</f>
+        <v>46.666666666666664</v>
+      </c>
+      <c r="AG339" s="110">
+        <f t="shared" ref="AG339:AG341" si="54">(B339-AF339)/AF339</f>
+        <v>0.60714285714285721</v>
+      </c>
+    </row>
+    <row r="340" spans="1:33">
+      <c r="A340" s="37">
+        <v>44676</v>
+      </c>
+      <c r="B340" s="38">
+        <v>25</v>
+      </c>
+      <c r="C340" s="38">
+        <v>13</v>
+      </c>
+      <c r="D340" s="38">
+        <v>-677</v>
+      </c>
+      <c r="E340" s="38">
+        <v>-569</v>
+      </c>
+      <c r="F340" s="38">
+        <v>-3993</v>
+      </c>
+      <c r="G340" s="38">
+        <v>-3781</v>
+      </c>
+      <c r="H340" s="38">
+        <v>-250</v>
+      </c>
+      <c r="I340" s="39">
+        <f t="shared" si="26"/>
+        <v>65.789473684210535</v>
+      </c>
+      <c r="J340" s="39">
+        <v>-2.72</v>
+      </c>
+      <c r="K340" s="39">
+        <v>-4.0199999999999996</v>
+      </c>
+      <c r="T340" s="94">
+        <v>4</v>
+      </c>
+      <c r="U340" s="43">
+        <v>3</v>
+      </c>
+      <c r="AF340" s="109">
+        <f t="shared" si="53"/>
+        <v>53</v>
+      </c>
+      <c r="AG340" s="110">
+        <f t="shared" si="54"/>
+        <v>-0.52830188679245282</v>
+      </c>
+    </row>
+    <row r="341" spans="1:33">
+      <c r="A341" s="37">
+        <v>44677</v>
+      </c>
+      <c r="B341" s="38">
+        <v>42</v>
+      </c>
+      <c r="C341" s="38">
+        <v>41</v>
+      </c>
+      <c r="D341" s="38">
+        <v>-272</v>
+      </c>
+      <c r="E341" s="38">
+        <v>-184</v>
+      </c>
+      <c r="F341" s="38">
+        <v>-2044</v>
+      </c>
+      <c r="G341" s="38">
+        <v>-1506</v>
+      </c>
+      <c r="H341" s="38">
+        <v>-250</v>
+      </c>
+      <c r="I341" s="39">
+        <f t="shared" ref="I341:I344" si="55">B341/(B341+C341)*100</f>
+        <v>50.602409638554214</v>
+      </c>
+      <c r="J341" s="39">
+        <v>0.09</v>
+      </c>
+      <c r="K341" s="39">
+        <v>-0.25</v>
+      </c>
+      <c r="T341" s="94">
+        <v>3</v>
+      </c>
+      <c r="U341" s="43">
+        <v>2</v>
+      </c>
+      <c r="AF341" s="109">
+        <f t="shared" si="53"/>
+        <v>44</v>
+      </c>
+      <c r="AG341" s="110">
+        <f t="shared" si="54"/>
+        <v>-4.5454545454545456E-2</v>
+      </c>
+    </row>
+    <row r="342" spans="1:33">
+      <c r="A342" s="37">
+        <v>44678</v>
+      </c>
+      <c r="B342" s="38">
+        <v>137</v>
+      </c>
+      <c r="C342" s="38">
+        <v>39</v>
+      </c>
+      <c r="D342" s="38">
+        <v>-148</v>
+      </c>
+      <c r="E342" s="38">
+        <v>-20</v>
+      </c>
+      <c r="F342" s="38">
+        <v>-1271</v>
+      </c>
+      <c r="G342" s="38">
+        <v>-154</v>
+      </c>
+      <c r="H342" s="38">
+        <v>-250</v>
+      </c>
+      <c r="I342" s="39">
+        <f t="shared" si="55"/>
+        <v>77.840909090909093</v>
+      </c>
+      <c r="J342" s="39">
+        <v>3.67</v>
+      </c>
+      <c r="K342" s="39">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="T342" s="94">
+        <v>4</v>
+      </c>
+      <c r="U342" s="43">
+        <v>3</v>
+      </c>
+      <c r="AF342" s="109">
+        <f t="shared" ref="AF342:AF344" si="56">(B339+B340+B341)/3</f>
+        <v>47.333333333333336</v>
+      </c>
+      <c r="AG342" s="110">
+        <f t="shared" ref="AG342:AG344" si="57">(B342-AF342)/AF342</f>
+        <v>1.8943661971830983</v>
+      </c>
+    </row>
+    <row r="343" spans="1:33">
+      <c r="A343" s="37">
+        <v>44679</v>
+      </c>
+      <c r="B343" s="38">
+        <v>68</v>
+      </c>
+      <c r="C343" s="38">
+        <v>21</v>
+      </c>
+      <c r="D343" s="38">
+        <v>-73</v>
+      </c>
+      <c r="E343" s="38">
+        <v>-24</v>
+      </c>
+      <c r="F343" s="38">
+        <v>-1334</v>
+      </c>
+      <c r="G343" s="38">
+        <v>-591</v>
+      </c>
+      <c r="H343" s="38">
+        <v>-250</v>
+      </c>
+      <c r="I343" s="39">
+        <f t="shared" si="55"/>
+        <v>76.404494382022463</v>
+      </c>
+      <c r="J343" s="39">
+        <v>3</v>
+      </c>
+      <c r="K343" s="39">
+        <v>2</v>
+      </c>
+      <c r="T343" s="94">
+        <v>5</v>
+      </c>
+      <c r="U343" s="43">
+        <v>3</v>
+      </c>
+      <c r="AF343" s="109">
+        <f t="shared" si="56"/>
+        <v>68</v>
+      </c>
+      <c r="AG343" s="110">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344" spans="1:33">
+      <c r="A344" s="37">
+        <v>44680</v>
+      </c>
+      <c r="B344" s="38">
+        <v>214</v>
+      </c>
+      <c r="C344" s="38">
+        <v>31</v>
+      </c>
+      <c r="D344" s="38">
+        <v>-18</v>
+      </c>
+      <c r="E344" s="38">
+        <v>0</v>
+      </c>
+      <c r="F344" s="38">
+        <v>-185</v>
+      </c>
+      <c r="G344" s="38">
+        <v>-31</v>
+      </c>
+      <c r="H344" s="38">
+        <v>-250</v>
+      </c>
+      <c r="I344" s="39">
+        <f t="shared" si="55"/>
+        <v>87.34693877551021</v>
+      </c>
+      <c r="J344" s="39">
+        <v>5.59</v>
+      </c>
+      <c r="K344" s="39">
+        <v>4.6100000000000003</v>
+      </c>
+      <c r="T344" s="94">
+        <v>6</v>
+      </c>
+      <c r="U344" s="43">
+        <v>4</v>
+      </c>
+      <c r="AF344" s="109">
+        <f t="shared" si="56"/>
+        <v>82.333333333333329</v>
+      </c>
+      <c r="AG344" s="110">
+        <f t="shared" si="57"/>
+        <v>1.59919028340081</v>
       </c>
     </row>
   </sheetData>
@@ -39447,7 +40089,7 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>I1:I1048576</xm:sqref>
+          <xm:sqref>J342 I1:I1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="7" id="{5668E6E0-C4AC-C442-9BCB-A9B3CB042970}">
@@ -39469,82 +40111,6 @@
           <xm:sqref>B1:B327 B330:B1048576 C328</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="5" id="{CC481063-6BD0-3947-B031-AA136F500496}">
-            <x14:iconSet iconSet="3Arrows" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>-38</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>-10</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>D1:D327 D330:D333 D335:D1048576 E334 E328</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="4" id="{DF774614-C12F-4C4F-9792-6234D19AF46D}">
-            <x14:iconSet iconSet="3Arrows" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>-20</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>-4</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>E1:E327 E330:E333 E335:E1048576 F334 F328</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="3" id="{8CB41595-F9EE-3547-A26F-50C5E7A82163}">
-            <x14:iconSet iconSet="3Arrows" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>-470</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>-200</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>F1:F327 F330:F333 F335:F1048576</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="2" id="{FF4E5384-FA77-554B-A82C-5F6FE16203A1}">
-            <x14:iconSet iconSet="3Arrows" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>-450</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>-50</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>G1:G328 G330:G1048576</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="1" id="{39F9903C-C6F9-E74E-A92D-D03599FF392A}">
             <x14:iconSet iconSet="3Arrows" custom="1">
               <x14:cfvo type="percent">
@@ -39562,6 +40128,82 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>D329:H329</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="13" id="{CC481063-6BD0-3947-B031-AA136F500496}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-38</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-10</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>D1:D327 D330:D333 E334 E328 D344:D1048576 D335:D342</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="20" id="{DF774614-C12F-4C4F-9792-6234D19AF46D}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-20</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-4</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>E1:E327 E330:E333 F334 F328 E344:E1048576 E335:E342</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="27" id="{8CB41595-F9EE-3547-A26F-50C5E7A82163}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-470</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-200</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>F1:F327 F330:F333 F344:F1048576 F335:F342</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="32" id="{FF4E5384-FA77-554B-A82C-5F6FE16203A1}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-450</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-50</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>G1:G328 G344:G1048576 G330:G342</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>